<commit_message>
changes made to test data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -142,10 +142,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -184,9 +184,107 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,15 +297,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,104 +316,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -328,187 +328,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,39 +519,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -570,17 +537,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,147 +604,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Completed add new opportunity script and test data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755"/>
+    <workbookView windowHeight="13960" tabRatio="755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
-    <sheet name="DemoTest" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="NewOpportunityTest" sheetId="3" r:id="rId3"/>
+    <sheet name="DashboardTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
   <si>
     <t>Parameters</t>
   </si>
@@ -131,10 +133,52 @@
     <t>Ashisht@plasmacomp.com,Plasma2!</t>
   </si>
   <si>
-    <t>verifyDashboard</t>
-  </si>
-  <si>
-    <t>skip</t>
+    <t>verifyNewOpportunityNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunityHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifySalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewOpprtunityCreation</t>
+  </si>
+  <si>
+    <t>verifyNewOpprtunity</t>
+  </si>
+  <si>
+    <t>verifyOpprtunities</t>
+  </si>
+  <si>
+    <t>verifyNewContract</t>
+  </si>
+  <si>
+    <t>verifyContracts</t>
+  </si>
+  <si>
+    <t>verifySearch</t>
+  </si>
+  <si>
+    <t>verifyHamburger</t>
+  </si>
+  <si>
+    <t>verifyDashboardHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyProfileIcon</t>
   </si>
 </sst>
 </file>
@@ -142,10 +186,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -176,47 +220,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,8 +280,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -237,44 +327,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -288,32 +341,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,13 +372,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,7 +516,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,157 +552,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,11 +590,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,6 +631,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -584,192 +663,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -777,9 +821,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1180,7 +1221,7 @@
   <sheetPr/>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1193,15 +1234,15 @@
   </cols>
   <sheetData>
     <row r="1" ht="22" spans="1:2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="22" spans="1:2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1209,7 +1250,7 @@
       </c>
     </row>
     <row r="3" ht="22" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1217,7 +1258,7 @@
       </c>
     </row>
     <row r="4" ht="22" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1225,7 +1266,7 @@
       </c>
     </row>
     <row r="5" ht="22" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
@@ -1233,7 +1274,7 @@
       </c>
     </row>
     <row r="6" ht="22" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1241,7 +1282,7 @@
       </c>
     </row>
     <row r="7" ht="22" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2">
@@ -1249,7 +1290,7 @@
       </c>
     </row>
     <row r="8" ht="22" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1257,7 +1298,7 @@
       </c>
     </row>
     <row r="9" ht="22" spans="1:2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
@@ -1265,7 +1306,7 @@
       </c>
     </row>
     <row r="10" ht="22" spans="1:2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1273,7 +1314,7 @@
       </c>
     </row>
     <row r="11" ht="22" spans="1:2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1281,7 +1322,7 @@
       </c>
     </row>
     <row r="12" ht="22" spans="1:2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1289,7 +1330,7 @@
       </c>
     </row>
     <row r="13" ht="22" spans="1:2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1297,7 +1338,7 @@
       </c>
     </row>
     <row r="14" ht="22" spans="1:2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1305,15 +1346,15 @@
       </c>
     </row>
     <row r="15" ht="22" spans="1:2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="b">
+      <c r="B15" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" ht="22" spans="1:2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1321,7 +1362,7 @@
       </c>
     </row>
     <row r="17" ht="22" spans="1:2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1329,7 +1370,7 @@
       </c>
     </row>
     <row r="18" ht="22" spans="1:2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1337,7 +1378,7 @@
       </c>
     </row>
     <row r="19" ht="22" spans="1:2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1362,13 +1403,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1397,15 +1438,6 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Ashisht@plasmacomp.com,Plasma2!" tooltip="mailto:Ashisht@plasmacomp.com,Plasma2!"/>
@@ -1414,4 +1446,214 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" ht="22" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" ht="22" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" ht="22" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="22" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" ht="22" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" ht="22" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" ht="22" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" ht="22" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="22" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" ht="22" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to test data file
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755" activeTab="1"/>
+    <workbookView windowHeight="13960" tabRatio="755"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>deviceNameIOS</t>
   </si>
   <si>
-    <t>iPad Pro (11-inch)</t>
+    <t>iPad Air (3rd generation)</t>
   </si>
   <si>
     <t>platformVersionIOS</t>
@@ -67,7 +67,7 @@
     <t>ipaFileName</t>
   </si>
   <si>
-    <t>/Users/plasmauser/Desktop/Landmark.app</t>
+    <t>/Users/macbookpro/Documents/Landmark_app/Landmark.app</t>
   </si>
   <si>
     <t>udid</t>
@@ -186,10 +186,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -220,31 +220,129 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,105 +357,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,13 +372,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,7 +528,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,151 +552,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,51 +566,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -631,24 +590,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -663,150 +604,209 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1221,8 +1221,8 @@
   <sheetPr/>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1405,7 +1405,7 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
splitted new opportunity creation flow
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755" activeTab="3"/>
+    <workbookView windowHeight="13960" tabRatio="755"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
   <si>
     <t>Parameters</t>
   </si>
@@ -154,7 +154,31 @@
     <t>verifyAttachmentsLabel</t>
   </si>
   <si>
-    <t>verifyNewOpprtunityCreation</t>
+    <t>verifyAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyAddVendorInfo</t>
+  </si>
+  <si>
+    <t>verifyAddLotsInfo</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageHeaderLabels</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageValues</t>
+  </si>
+  <si>
+    <t>verifyAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyAttachments</t>
+  </si>
+  <si>
+    <t>verifyAddNotes</t>
+  </si>
+  <si>
+    <t>verifyNotes</t>
   </si>
   <si>
     <t>verifyNewOpportunity</t>
@@ -186,10 +210,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -221,14 +245,135 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,127 +386,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -378,181 +402,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,15 +595,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,17 +629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -642,9 +646,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,150 +678,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1221,7 +1245,7 @@
   <sheetPr/>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1451,10 +1475,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1547,6 +1571,70 @@
       </c>
       <c r="C9" s="4"/>
     </row>
+    <row r="10" ht="22" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" ht="22" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" ht="22" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" ht="22" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="22" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" ht="22" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" ht="22" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" ht="22" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1558,7 +1646,7 @@
   <sheetPr/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1582,7 +1670,7 @@
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
@@ -1591,7 +1679,7 @@
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>36</v>
@@ -1600,7 +1688,7 @@
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -1609,7 +1697,7 @@
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>36</v>
@@ -1618,7 +1706,7 @@
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>36</v>
@@ -1627,7 +1715,7 @@
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>36</v>
@@ -1636,7 +1724,7 @@
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>36</v>
@@ -1645,7 +1733,7 @@
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
completed all test cases upto opportunity creation
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -58,7 +58,7 @@
     <t>deviceNameIOS</t>
   </si>
   <si>
-    <t>iPad Air (3rd generation)</t>
+    <t>iPad Air</t>
   </si>
   <si>
     <t>platformVersionIOS</t>
@@ -67,7 +67,7 @@
     <t>ipaFileName</t>
   </si>
   <si>
-    <t>/Users/macbookpro/Documents/Landmark_app/Landmark.app</t>
+    <t>/Users/ataurrahman/Documents/Landmark.app</t>
   </si>
   <si>
     <t>udid</t>
@@ -210,10 +210,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -245,7 +245,90 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,9 +342,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,29 +368,6 @@
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,21 +379,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,65 +386,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -396,145 +396,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,37 +576,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,6 +595,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,26 +653,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -687,150 +676,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1326,7 +1326,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>13.4</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="10" ht="22" spans="1:2">

</xml_diff>

<commit_message>
Last commit from TTN mac
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755"/>
+    <workbookView windowHeight="13960" tabRatio="755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
     <sheet name="NewOpportunityTest" sheetId="3" r:id="rId3"/>
     <sheet name="DashboardTest" sheetId="4" r:id="rId4"/>
+    <sheet name="ListingInfoTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66">
   <si>
     <t>Parameters</t>
   </si>
@@ -203,6 +204,18 @@
   </si>
   <si>
     <t>verifyProfileIcon</t>
+  </si>
+  <si>
+    <t>verifyListingTypeOptions</t>
+  </si>
+  <si>
+    <t>verifyClassifiedListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingType</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelection</t>
   </si>
 </sst>
 </file>
@@ -210,9 +223,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -244,6 +257,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -259,6 +280,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -266,8 +348,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,112 +399,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -396,187 +409,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,69 +600,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -671,8 +621,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,150 +667,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1245,7 +1258,7 @@
   <sheetPr/>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1647,7 +1660,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A1" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1744,4 +1757,73 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" ht="22" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed listing info page test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755" activeTab="4"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
   <si>
     <t>Parameters</t>
   </si>
@@ -216,6 +216,27 @@
   </si>
   <si>
     <t>verifyListingTypeSelection</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigation</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetails</t>
   </si>
 </sst>
 </file>
@@ -223,9 +244,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -257,6 +278,126 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -266,17 +407,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -287,118 +420,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -409,61 +430,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,121 +604,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,45 +621,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -659,11 +641,33 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,9 +689,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -695,8 +701,23 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,145 +726,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1762,13 +1783,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1822,6 +1843,69 @@
       </c>
       <c r="C5" s="4"/>
     </row>
+    <row r="6" ht="22" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" ht="22" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="22" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" ht="22" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" ht="22" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" ht="22" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" ht="22" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added publish listing script
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74">
   <si>
     <t>Parameters</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>verifyFillingDeliveryDetails</t>
+  </si>
+  <si>
+    <t>verifyPublishListing</t>
   </si>
 </sst>
 </file>
@@ -244,9 +247,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -285,6 +288,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -295,14 +358,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,60 +379,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,44 +423,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -430,6 +433,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -442,13 +469,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,157 +613,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,6 +624,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -642,82 +719,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,142 +729,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1783,7 +1786,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -1906,6 +1909,15 @@
       </c>
       <c r="C12" s="4"/>
     </row>
+    <row r="13" ht="22" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
completed new opportunity scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" activeTab="4"/>
+    <workbookView windowHeight="13960" tabRatio="755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="NewOpportunityTest" sheetId="3" r:id="rId3"/>
     <sheet name="DashboardTest" sheetId="4" r:id="rId4"/>
     <sheet name="ListingInfoTest" sheetId="5" r:id="rId5"/>
+    <sheet name="ListingInfoClassifiedTest" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
   <si>
     <t>Parameters</t>
   </si>
@@ -59,7 +60,7 @@
     <t>deviceNameIOS</t>
   </si>
   <si>
-    <t>iPad Air</t>
+    <t>iPad Air (3rd generation)</t>
   </si>
   <si>
     <t>platformVersionIOS</t>
@@ -239,7 +240,31 @@
     <t>verifyFillingDeliveryDetails</t>
   </si>
   <si>
+    <t>verifyFillingLiveWeightDetails</t>
+  </si>
+  <si>
     <t>verifyPublishListing</t>
+  </si>
+  <si>
+    <t>CreateOpportunityForClassified</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelectionClassified</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigationClassified</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListing</t>
   </si>
 </sst>
 </file>
@@ -247,10 +272,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -295,8 +320,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,6 +336,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -318,31 +390,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,6 +413,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,64 +443,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -439,181 +464,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,11 +652,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,26 +700,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -682,21 +711,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,6 +732,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -729,139 +754,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1363,7 +1388,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>11.4</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="10" ht="22" spans="1:2">
@@ -1466,8 +1491,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1515,7 +1540,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1684,7 +1709,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1786,10 +1811,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1918,6 +1943,111 @@
       </c>
       <c r="C13" s="4"/>
     </row>
+    <row r="14" ht="22" spans="1:3">
+      <c r="A14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" ht="22" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" ht="22" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" ht="22" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="22" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added Econtract test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755" activeTab="1"/>
+    <workbookView windowHeight="13960" tabRatio="755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="DashboardTest" sheetId="4" r:id="rId4"/>
     <sheet name="ListingInfoTest" sheetId="5" r:id="rId5"/>
     <sheet name="ListingInfoClassifiedTest" sheetId="6" r:id="rId6"/>
+    <sheet name="NewContractTest" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86">
   <si>
     <t>Parameters</t>
   </si>
@@ -102,7 +103,7 @@
     <t>mailRecipient</t>
   </si>
   <si>
-    <t>ataur.rahman@plasmacomp.com</t>
+    <t>ashisht@plasmacomp.com</t>
   </si>
   <si>
     <t>raiseIssue</t>
@@ -129,126 +130,129 @@
     <t>loginTest</t>
   </si>
   <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>Ashisht@plasmacomp.com,Plasma2!</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunityNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunityHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifySalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyAddVendorInfo</t>
+  </si>
+  <si>
+    <t>verifyAddLotsInfo</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageHeaderLabels</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageValues</t>
+  </si>
+  <si>
+    <t>verifyAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyAttachments</t>
+  </si>
+  <si>
+    <t>verifyAddNotes</t>
+  </si>
+  <si>
+    <t>verifyNotes</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunity</t>
+  </si>
+  <si>
+    <t>verifyOpportunities</t>
+  </si>
+  <si>
+    <t>verifyNewContract</t>
+  </si>
+  <si>
+    <t>verifyContracts</t>
+  </si>
+  <si>
+    <t>verifySearch</t>
+  </si>
+  <si>
+    <t>verifyHamburger</t>
+  </si>
+  <si>
+    <t>verifyDashboardHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyProfileIcon</t>
+  </si>
+  <si>
+    <t>verifyListingTypeOptions</t>
+  </si>
+  <si>
+    <t>verifyClassifiedListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingType</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelection</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigation</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingLiveWeightDetails</t>
+  </si>
+  <si>
+    <t>verifyPublishListing</t>
+  </si>
+  <si>
+    <t>CreateOpportunityForClassified</t>
+  </si>
+  <si>
     <t>run</t>
   </si>
   <si>
-    <t>Ashisht@plasmacomp.com,Plasma2!</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunityNavigation</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunityHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifySalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyLotsLabel</t>
-  </si>
-  <si>
-    <t>verifyNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyAddSalesInformation</t>
-  </si>
-  <si>
-    <t>verifyAddVendorInfo</t>
-  </si>
-  <si>
-    <t>verifyAddLotsInfo</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageHeaderLabels</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageValues</t>
-  </si>
-  <si>
-    <t>verifyAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyAttachments</t>
-  </si>
-  <si>
-    <t>verifyAddNotes</t>
-  </si>
-  <si>
-    <t>verifyNotes</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunity</t>
-  </si>
-  <si>
-    <t>verifyOpportunities</t>
-  </si>
-  <si>
-    <t>verifyNewContract</t>
-  </si>
-  <si>
-    <t>verifyContracts</t>
-  </si>
-  <si>
-    <t>verifySearch</t>
-  </si>
-  <si>
-    <t>verifyHamburger</t>
-  </si>
-  <si>
-    <t>verifyDashboardHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyProfileIcon</t>
-  </si>
-  <si>
-    <t>verifyListingTypeOptions</t>
-  </si>
-  <si>
-    <t>verifyClassifiedListingType</t>
-  </si>
-  <si>
-    <t>verifyBidAndOfferListingType</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelection</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigation</t>
-  </si>
-  <si>
-    <t>verifyFillingListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingWeightsSummaryDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingAssessmentOverviewDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingBreedingOverviewDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingHealthVetDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingDeliveryDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingLiveWeightDetails</t>
-  </si>
-  <si>
-    <t>verifyPublishListing</t>
-  </si>
-  <si>
-    <t>CreateOpportunityForClassified</t>
-  </si>
-  <si>
     <t>verifyListingTypeSelectionClassified</t>
   </si>
   <si>
@@ -265,6 +269,15 @@
   </si>
   <si>
     <t>verifyClassifiedPublishListing</t>
+  </si>
+  <si>
+    <t>verifyOpportunityIdNavigationFromGridPage</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigationFromListingPage</t>
+  </si>
+  <si>
+    <t>verifyFillingNewContract</t>
   </si>
 </sst>
 </file>
@@ -272,10 +285,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -309,12 +322,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,6 +349,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -336,37 +409,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -375,6 +417,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -382,11 +425,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -399,55 +456,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -458,6 +471,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -470,49 +489,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,121 +639,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,15 +684,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -696,6 +700,35 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -729,170 +762,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1308,7 +1321,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1478,7 +1491,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" display="ataur.rahman@plasmacomp.com" tooltip="mailto:ataur.rahman@plasmacomp.com"/>
+    <hyperlink ref="B16" r:id="rId1" display="ashisht@plasmacomp.com" tooltip="mailto:ashisht@plasmacomp.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1491,8 +1504,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1540,7 +1553,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1709,7 +1722,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1814,7 +1827,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
@@ -1963,8 +1976,8 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -1990,63 +2003,123 @@
         <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
fixed issues in econtract script and made other changes as per new build
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13960" tabRatio="755" activeTab="5"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -130,15 +130,18 @@
     <t>loginTest</t>
   </si>
   <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Ashisht@plasmacomp.com,Plasma2!</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunityNavigation</t>
+  </si>
+  <si>
     <t>skip</t>
   </si>
   <si>
-    <t>Ashisht@plasmacomp.com,Plasma2!</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunityNavigation</t>
-  </si>
-  <si>
     <t>verifyNewOpportunityHeaderLabel</t>
   </si>
   <si>
@@ -248,9 +251,6 @@
   </si>
   <si>
     <t>CreateOpportunityForClassified</t>
-  </si>
-  <si>
-    <t>run</t>
   </si>
   <si>
     <t>verifyListingTypeSelectionClassified</t>
@@ -285,10 +285,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -322,12 +322,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,14 +349,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -357,8 +357,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,32 +395,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -409,8 +432,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -431,36 +461,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -471,37 +471,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,7 +597,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,133 +651,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,7 +684,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,11 +704,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -732,180 +762,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1579,135 +1579,135 @@
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" ht="22" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" ht="22" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" ht="22" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" ht="22" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" ht="22" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" ht="22" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" ht="22" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" ht="22" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1745,73 +1745,73 @@
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -1850,118 +1850,118 @@
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4"/>
     </row>
     <row r="10" ht="22" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4"/>
     </row>
     <row r="11" ht="22" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" ht="22" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" ht="22" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" ht="22" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -1976,8 +1976,8 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -2000,10 +2000,10 @@
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -2012,7 +2012,7 @@
         <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -2021,7 +2021,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -2030,7 +2030,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -2039,7 +2039,7 @@
         <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4"/>
     </row>
@@ -2048,7 +2048,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -2057,7 +2057,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -2072,8 +2072,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -2099,7 +2099,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -2108,7 +2108,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -2117,7 +2117,7 @@
         <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4"/>
     </row>

</xml_diff>

<commit_message>
Test data moved to test data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="ListingInfoTest" sheetId="5" r:id="rId5"/>
     <sheet name="ListingInfoClassifiedTest" sheetId="6" r:id="rId6"/>
     <sheet name="NewContractTest" sheetId="7" r:id="rId7"/>
+    <sheet name="NewContractDashboardTest" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144">
   <si>
     <t>Parameters</t>
   </si>
@@ -127,6 +128,9 @@
     <t>Params</t>
   </si>
   <si>
+    <t>Remarks</t>
+  </si>
+  <si>
     <t>loginTest</t>
   </si>
   <si>
@@ -154,6 +158,12 @@
     <t>verifyLotsLabel</t>
   </si>
   <si>
+    <t>Agent settlement,Alexandra,June,8,2020</t>
+  </si>
+  <si>
+    <t>salesType,branchName,month,day,year</t>
+  </si>
+  <si>
     <t>verifyNotesLabel</t>
   </si>
   <si>
@@ -166,15 +176,33 @@
     <t>verifyAddVendorInfo</t>
   </si>
   <si>
+    <t>A Rigano Farms</t>
+  </si>
+  <si>
+    <t>vendorName</t>
+  </si>
+  <si>
     <t>verifyAddLotsInfo</t>
   </si>
   <si>
+    <t>10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
+  </si>
+  <si>
     <t>verifyLotSummaryPageHeaderLabels</t>
   </si>
   <si>
     <t>verifyLotSummaryPageValues</t>
   </si>
   <si>
+    <t>10,10,0</t>
+  </si>
+  <si>
+    <t>quantity,price,weight</t>
+  </si>
+  <si>
     <t>verifyAddAttachments</t>
   </si>
   <si>
@@ -184,6 +212,12 @@
     <t>verifyAddNotes</t>
   </si>
   <si>
+    <t>Automation note</t>
+  </si>
+  <si>
+    <t>noteText</t>
+  </si>
+  <si>
     <t>verifyNotes</t>
   </si>
   <si>
@@ -223,36 +257,84 @@
     <t>verifyListingTypeSelection</t>
   </si>
   <si>
+    <t>Online,Dairy</t>
+  </si>
+  <si>
+    <t>transactionType,saleType</t>
+  </si>
+  <si>
     <t>verifyListingInfoNavigation</t>
   </si>
   <si>
     <t>verifyFillingListingOverviewDetails</t>
   </si>
   <si>
+    <t>24 hours,3 hours,200,Test Description,215,BRISBANE</t>
+  </si>
+  <si>
+    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
+  </si>
+  <si>
     <t>verifyFillingWeightsSummaryDetails</t>
   </si>
   <si>
+    <t>2,4,12,5,4,10</t>
+  </si>
+  <si>
+    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
+  </si>
+  <si>
     <t>verifyFillingAssessmentOverviewDetails</t>
   </si>
   <si>
+    <t>Small,Prime,Test comment</t>
+  </si>
+  <si>
+    <t>frame,condition,agentComment</t>
+  </si>
+  <si>
     <t>verifyFillingBreedingOverviewDetails</t>
   </si>
   <si>
+    <t>Yes,Quiet</t>
+  </si>
+  <si>
+    <t>vendorBred,temperament</t>
+  </si>
+  <si>
     <t>verifyFillingHealthVetDetails</t>
   </si>
   <si>
+    <t>Yes,Yes</t>
+  </si>
+  <si>
+    <t>hgpTreated,withinWithholdingPeriod</t>
+  </si>
+  <si>
     <t>verifyFillingDeliveryDetails</t>
   </si>
   <si>
     <t>verifyFillingLiveWeightDetails</t>
   </si>
   <si>
+    <t>20,Fat score 1 (0-2mm)</t>
+  </si>
+  <si>
+    <t>liveWeight,fatScore</t>
+  </si>
+  <si>
     <t>verifyPublishListing</t>
   </si>
   <si>
     <t>CreateOpportunityForClassified</t>
   </si>
   <si>
+    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
+  </si>
+  <si>
+    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
+  </si>
+  <si>
     <t>verifyListingTypeSelectionClassified</t>
   </si>
   <si>
@@ -262,9 +344,21 @@
     <t>verifyFillingClassifiedListingOverviewDetails</t>
   </si>
   <si>
+    <t>14 days,150,Test Description</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description</t>
+  </si>
+  <si>
     <t>verifyFillingClassifiedLotDetails</t>
   </si>
   <si>
+    <t>Polled,10,20</t>
+  </si>
+  <si>
+    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
+  </si>
+  <si>
     <t>verifyFillingClassifiedHealthVetDetails</t>
   </si>
   <si>
@@ -278,6 +372,87 @@
   </si>
   <si>
     <t>verifyFillingNewContract</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
+  </si>
+  <si>
+    <t>salesType,branchName,buyerName,deliveryPoint</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewContractHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractSalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyBuyerInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyDeliveryInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyAdditionalChargesLabel</t>
+  </si>
+  <si>
+    <t>verifyCommissionAndAgentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddVendorInfo</t>
+  </si>
+  <si>
+    <t>verifyAddBuyerInfo</t>
+  </si>
+  <si>
+    <t>AJ Pointon &amp; AW Pointon</t>
+  </si>
+  <si>
+    <t>buyerName</t>
+  </si>
+  <si>
+    <t>verifyAddDeliveryInfo</t>
+  </si>
+  <si>
+    <t>Test Delivery Point,June,12,2020</t>
+  </si>
+  <si>
+    <t>deliveryPoint,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddLotsInfo</t>
+  </si>
+  <si>
+    <t>verifyAddAdditionalCharges</t>
+  </si>
+  <si>
+    <t>verifyAddCommissionAndAgents</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachments</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddNotes</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotes</t>
   </si>
 </sst>
 </file>
@@ -285,8 +460,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -326,13 +501,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -341,11 +509,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,7 +526,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -381,17 +572,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,17 +624,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,29 +636,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -471,61 +646,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,121 +820,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,6 +864,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -700,6 +895,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,41 +929,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -767,142 +942,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1502,20 +1677,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="13.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="22" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1525,16 +1701,19 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1550,13 +1729,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1576,138 +1755,176 @@
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" ht="22" spans="1:3">
+    <row r="6" ht="22" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" ht="22" spans="1:2">
+    <row r="10" ht="22" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" ht="22" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" ht="22" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" ht="22" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="14" ht="22" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" ht="22" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" ht="22" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" ht="22" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" ht="22" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1719,20 +1936,21 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="13.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="22" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1742,76 +1960,79 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4"/>
     </row>
     <row r="5" ht="22" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" ht="22" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" ht="22" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -1824,20 +2045,21 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="83.984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="22" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1847,121 +2069,159 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" ht="22" spans="1:3">
+    <row r="5" ht="22" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" ht="22" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" ht="22" spans="1:3">
+    <row r="7" ht="22" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" ht="22" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" ht="22" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" ht="22" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" ht="22" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="12" ht="22" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" ht="22" spans="1:3">
+    <row r="13" ht="22" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" ht="22" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -1974,20 +2234,21 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="156.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="22" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1997,67 +2258,95 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" ht="22" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" ht="22" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" ht="22" spans="1:3">
+    <row r="5" ht="22" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" ht="22" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" ht="22" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" ht="22" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" ht="22" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -2070,20 +2359,21 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="65.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="13.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="22" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2093,33 +2383,302 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" ht="22" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" ht="22" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="22" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="137.6875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" ht="22" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="22" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4"/>
+    </row>
+    <row r="5" ht="22" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" ht="22" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" ht="22" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" ht="22" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" ht="22" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" ht="22" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" ht="22" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" ht="22" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" ht="22" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" ht="22" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" ht="22" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" ht="22" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" ht="22" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" ht="22" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" ht="22" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" ht="22" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" ht="22" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" ht="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Added conditional test scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="3" activeTab="7"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="ListingInfoClassifiedTest" sheetId="6" r:id="rId6"/>
     <sheet name="NewContractTest" sheetId="7" r:id="rId7"/>
     <sheet name="NewContractDashboardTest" sheetId="8" r:id="rId8"/>
+    <sheet name="NewOpportunityConditionalTest" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148">
   <si>
     <t>Parameters</t>
   </si>
@@ -453,6 +454,18 @@
   </si>
   <si>
     <t>verifyNewContractNotes</t>
+  </si>
+  <si>
+    <t>verifyValidateContract</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>signatureText</t>
+  </si>
+  <si>
+    <t>VerifyCreateNewOpportunityWithTwoLots</t>
   </si>
 </sst>
 </file>
@@ -460,10 +473,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -503,7 +516,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,14 +542,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -541,10 +561,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -563,34 +583,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -603,14 +599,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -631,7 +620,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -646,187 +659,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -840,17 +853,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -860,6 +873,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,23 +900,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -929,11 +936,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -942,142 +955,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1732,7 +1745,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -1939,7 +1952,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2362,7 +2375,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A1" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -2428,10 +2441,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2680,6 +2693,71 @@
         <v>64</v>
       </c>
     </row>
+    <row r="23" ht="22" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="4" max="4" width="13.1875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" ht="22" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
completed Lot conditional test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164">
   <si>
     <t>Parameters</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>verifyWeightValueOnLotGridPage</t>
+  </si>
+  <si>
+    <t>quantity,weight</t>
   </si>
   <si>
     <t>verifyAddingSecondLotInTheSameOpportunity</t>
@@ -518,10 +521,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -553,14 +556,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -580,18 +583,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -612,39 +608,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,7 +623,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -665,11 +636,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -681,10 +659,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -694,6 +681,22 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -704,187 +707,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,6 +898,62 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -917,71 +976,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -995,150 +989,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1791,7 +1794,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B3" sqref="B3:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2107,7 +2110,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2765,7 +2768,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2840,21 +2843,21 @@
         <v>147</v>
       </c>
       <c r="C5" s="4">
-        <v>15900</v>
+        <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" ht="22" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>151</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="7" ht="22" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>147</v>
@@ -2870,21 +2873,21 @@
     </row>
     <row r="8" ht="22" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>147</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" ht="22" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>147</v>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="10" ht="22" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
completed Sheep classified test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="755" firstSheet="5" activeTab="8"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <sheet name="NewContractTest" sheetId="7" r:id="rId7"/>
     <sheet name="NewContractDashboardTest" sheetId="8" r:id="rId8"/>
     <sheet name="NewOpportunityConditionalTest" sheetId="9" r:id="rId9"/>
+    <sheet name="ListingInfoSheepBidAndOfferTest" sheetId="10" r:id="rId10"/>
+    <sheet name="ListingInfoSheepClassified" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197">
   <si>
     <t>Parameters</t>
   </si>
@@ -135,15 +137,21 @@
     <t>loginTest</t>
   </si>
   <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Ashisht@plasmacomp.com,Plasma2!</t>
+  </si>
+  <si>
+    <t>Username, password</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunityNavigation</t>
+  </si>
+  <si>
     <t>skip</t>
   </si>
   <si>
-    <t>Ashisht@plasmacomp.com,Plasma2!</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunityNavigation</t>
-  </si>
-  <si>
     <t>verifyNewOpportunityHeaderLabel</t>
   </si>
   <si>
@@ -267,7 +275,7 @@
     <t>verifyFillingListingOverviewDetails</t>
   </si>
   <si>
-    <t>24 hours,3 hours,200,Test Description,215,BRISBANE</t>
+    <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
   </si>
   <si>
     <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
@@ -465,9 +473,6 @@
     <t>VerifyAddingSalesAndVendorInfo</t>
   </si>
   <si>
-    <t>run</t>
-  </si>
-  <si>
     <t>A Rigano</t>
   </si>
   <si>
@@ -514,6 +519,102 @@
   </si>
   <si>
     <t>verifyEnabledListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingTypeSelection</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetailsForSheep</t>
+  </si>
+  <si>
+    <t>Test Comment</t>
+  </si>
+  <si>
+    <t>agentComment</t>
+  </si>
+  <si>
+    <t>verifyFillingLambsAtFootDetailsForSheep</t>
+  </si>
+  <si>
+    <t>6,Test,4</t>
+  </si>
+  <si>
+    <t>numberOfLambsAtFoot,lambsAtFootSiredBy,ageOfLambs</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetailsForSheep</t>
+  </si>
+  <si>
+    <t>Yes,Yes,Yes</t>
+  </si>
+  <si>
+    <t>vendorBred,sheddingBreed,anyKnownContactWithSheddingBreed</t>
+  </si>
+  <si>
+    <t>verifyFillingWoolSkinDetailsForSheep</t>
+  </si>
+  <si>
+    <t>08 Aug 2020,Light,Medium</t>
+  </si>
+  <si>
+    <t>lastShearingDate,degreeOfBurr,degreeOfSeed</t>
+  </si>
+  <si>
+    <t>verifyFillingJoiningDetailsForSheep</t>
+  </si>
+  <si>
+    <t>numberOfHeadScanned</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingAccreditationDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingLiveWeightDetailsForSheep</t>
+  </si>
+  <si>
+    <t>20,12,Fat score 1 (0-2mm)</t>
+  </si>
+  <si>
+    <t>verifyPublishListingForSheep</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelectionClassifiedSheep</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigationClassifiedSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetailsSheep</t>
+  </si>
+  <si>
+    <t>14 days,150,Test Description,BEULAH</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description,town</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetailsSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetailsSheep</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedAccreditationDetailsForSheep</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListingSheep</t>
   </si>
 </sst>
 </file>
@@ -521,12 +622,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -535,16 +636,30 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -563,14 +678,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,16 +708,47 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,7 +763,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,11 +783,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -636,63 +805,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,7 +822,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -719,13 +966,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,31 +984,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,85 +996,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,43 +1006,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -912,32 +1051,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -974,9 +1087,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,166 +1133,169 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1558,166 +1691,166 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="68.2890625" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="44.6875" customWidth="1"/>
     <col min="3" max="3" width="49.140625" customWidth="1"/>
     <col min="4" max="4" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:2">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="14.8" spans="1:2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:2">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="14.8" spans="1:2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="22" spans="1:2">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="14.8" spans="1:2">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="22" spans="1:2">
-      <c r="A4" s="6" t="s">
+    <row r="4" ht="14.8" spans="1:2">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="22" spans="1:2">
-      <c r="A5" s="6" t="s">
+    <row r="5" ht="14.8" spans="1:2">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="22" spans="1:2">
-      <c r="A6" s="6" t="s">
+    <row r="6" ht="14.8" spans="1:2">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="22" spans="1:2">
-      <c r="A7" s="6" t="s">
+    <row r="7" ht="14.8" spans="1:2">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>4723</v>
       </c>
     </row>
-    <row r="8" ht="22" spans="1:2">
-      <c r="A8" s="6" t="s">
+    <row r="8" ht="14.8" spans="1:2">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" ht="22" spans="1:2">
-      <c r="A9" s="6" t="s">
+    <row r="9" ht="14.8" spans="1:2">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
         <v>13.4</v>
       </c>
     </row>
-    <row r="10" ht="22" spans="1:2">
-      <c r="A10" s="6" t="s">
+    <row r="10" ht="14.8" spans="1:2">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" ht="22" spans="1:2">
-      <c r="A11" s="6" t="s">
+    <row r="11" ht="14.8" spans="1:2">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="22" spans="1:2">
-      <c r="A12" s="6" t="s">
+    <row r="12" ht="14.8" spans="1:2">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="22" spans="1:2">
-      <c r="A13" s="6" t="s">
+    <row r="13" ht="14.8" spans="1:2">
+      <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" ht="22" spans="1:2">
-      <c r="A14" s="6" t="s">
+    <row r="14" ht="14.8" spans="1:2">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" ht="22" spans="1:2">
-      <c r="A15" s="6" t="s">
+    <row r="15" ht="14.8" spans="1:2">
+      <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="b">
+      <c r="B15" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" ht="22" spans="1:2">
-      <c r="A16" s="6" t="s">
+    <row r="16" ht="14.8" spans="1:2">
+      <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" ht="22" spans="1:2">
-      <c r="A17" s="6" t="s">
+    <row r="17" ht="14.8" spans="1:2">
+      <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="22" spans="1:2">
-      <c r="A18" s="6" t="s">
+    <row r="18" ht="14.8" spans="1:2">
+      <c r="A18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" ht="22" spans="1:2">
-      <c r="A19" s="6" t="s">
+    <row r="19" ht="14.8" spans="1:2">
+      <c r="A19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1736,24 +1869,329 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="46.1875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
+    <col min="4" max="4" width="117.6875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="46.1875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
+    <col min="4" max="4" width="117.6875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="15.75" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="15.75" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="15.75" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" customWidth="1"/>
+    <col min="1" max="1" width="15.9375" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="31.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1767,15 +2205,18 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="15" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1794,17 +2235,18 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
+    <col min="1" max="1" width="35.0625" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="43.359375" customWidth="1"/>
+    <col min="4" max="4" width="91.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:3">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1814,179 +2256,190 @@
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" ht="22" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" ht="22" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" ht="22" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" ht="22" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" ht="22" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" ht="14.8" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" ht="22" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" ht="14.8" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" ht="22" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" ht="14.8" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" ht="22" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" ht="14.8" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" ht="22" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>56</v>
+    <row r="13" ht="14.8" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" ht="22" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" ht="14.8" spans="1:4">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" ht="22" spans="1:3">
-      <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" ht="14.8" spans="1:4">
+      <c r="A15" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" ht="22" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" ht="14.8" spans="1:4">
+      <c r="A16" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" ht="22" spans="1:4">
-      <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" ht="14.8" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2001,18 +2454,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" customWidth="1"/>
+    <col min="1" max="1" width="27.6875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2026,77 +2479,85 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>65</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" ht="22" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" ht="22" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" ht="22" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" ht="22" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" ht="22" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" ht="14.8" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2109,19 +2570,19 @@
   <sheetPr/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="83.984375" customWidth="1"/>
+    <col min="1" max="1" width="37.1875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="47.2578125" customWidth="1"/>
+    <col min="4" max="4" width="117.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2135,157 +2596,163 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>73</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" ht="22" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" ht="22" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" ht="22" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" ht="22" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" ht="22" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" ht="14.8" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" ht="22" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" ht="14.8" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" ht="22" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" ht="14.8" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" ht="22" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" ht="14.8" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" ht="22" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>96</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" ht="14.8" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" ht="22" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" ht="14.8" spans="1:4">
+      <c r="A14" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2298,19 +2765,19 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="156.375" customWidth="1"/>
+    <col min="1" max="1" width="41.1875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="68.8828125" customWidth="1"/>
+    <col min="4" max="4" width="112.4375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2324,93 +2791,95 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>100</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" ht="22" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" ht="22" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" ht="22" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" ht="22" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" ht="22" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>112</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2424,18 +2893,18 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="59.8125" customWidth="1"/>
+    <col min="4" max="4" width="46.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2449,36 +2918,38 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>113</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" ht="22" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2493,18 +2964,18 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="137.6875" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="46.9375" customWidth="1"/>
+    <col min="4" max="4" width="91.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2518,242 +2989,256 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>118</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" ht="22" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" ht="22" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>41</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" ht="22" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" ht="22" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" ht="22" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>123</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" ht="22" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" ht="22" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>125</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" ht="14.8" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" ht="22" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" ht="14.8" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" ht="22" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>41</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" ht="14.8" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" ht="22" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>41</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" ht="14.8" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" ht="22" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" ht="14.8" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" ht="22" spans="1:4">
-      <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" ht="14.8" spans="1:4">
+      <c r="A14" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" ht="22" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>131</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" ht="14.8" spans="1:4">
+      <c r="A15" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" ht="22" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" ht="14.8" spans="1:4">
+      <c r="A16" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" ht="22" spans="1:4">
-      <c r="A17" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" ht="14.8" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" ht="22" spans="1:3">
-      <c r="A18" s="2" t="s">
-        <v>138</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" ht="14.8" spans="1:4">
+      <c r="A18" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" ht="22" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>139</v>
+        <v>41</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" ht="14.8" spans="1:4">
+      <c r="A19" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" ht="22" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>140</v>
+        <v>41</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" ht="14.8" spans="1:4">
+      <c r="A20" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" ht="22" spans="1:4">
-      <c r="A21" s="2" t="s">
-        <v>141</v>
+        <v>41</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" ht="14.8" spans="1:4">
+      <c r="A21" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" ht="22" spans="1:4">
-      <c r="A22" s="2" t="s">
-        <v>142</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" ht="14.8" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" ht="22" spans="1:4">
-      <c r="A23" s="2" t="s">
-        <v>143</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" ht="14.8" spans="1:4">
+      <c r="A23" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2767,19 +3252,19 @@
   <sheetPr/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.8125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="70.2890625" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" customWidth="1"/>
+    <col min="3" max="3" width="22.5625" customWidth="1"/>
+    <col min="4" max="4" width="38.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" spans="1:4">
+    <row r="1" ht="14.8" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2793,113 +3278,119 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" ht="22" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>146</v>
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" ht="22" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>149</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" ht="14.8" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" ht="22" spans="1:4">
-      <c r="A4" s="2" t="s">
         <v>152</v>
       </c>
+    </row>
+    <row r="4" ht="14.8" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3">
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" ht="22" spans="1:4">
-      <c r="A5" s="2" t="s">
         <v>154</v>
       </c>
+    </row>
+    <row r="5" ht="14.8" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="4">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5">
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" ht="22" spans="1:4">
-      <c r="A6" s="2" t="s">
         <v>156</v>
       </c>
+    </row>
+    <row r="6" ht="14.8" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" ht="22" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" ht="14.8" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" ht="22" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>159</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" ht="14.8" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" ht="22" spans="1:2">
-      <c r="A9" s="2" t="s">
         <v>162</v>
       </c>
+    </row>
+    <row r="9" ht="14.8" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" ht="22" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>163</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" ht="14.8" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>147</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
made changes as per new build after removal of SSO
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="7" activeTab="9"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <t>ipaFileName</t>
   </si>
   <si>
-    <t>/Users/ataurrahman/Documents/Landmark.app</t>
+    <t>/Users/ataurrahman/Documents/Nutrien.app</t>
   </si>
   <si>
     <t>udid</t>
@@ -149,109 +149,109 @@
     <t>verifyNewOpportunityNavigation</t>
   </si>
   <si>
+    <t>verifyNewOpportunityHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifySalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyLotsLabel</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,June,8,2020</t>
+  </si>
+  <si>
+    <t>salesType,branchName,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyAddVendorInfo</t>
+  </si>
+  <si>
+    <t>A Rigano Farms</t>
+  </si>
+  <si>
+    <t>vendorName</t>
+  </si>
+  <si>
+    <t>verifyAddLotsInfo</t>
+  </si>
+  <si>
+    <t>10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageHeaderLabels</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageValues</t>
+  </si>
+  <si>
+    <t>10,10,0</t>
+  </si>
+  <si>
+    <t>quantity,price,weight</t>
+  </si>
+  <si>
+    <t>verifyAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyAttachments</t>
+  </si>
+  <si>
+    <t>verifyAddNotes</t>
+  </si>
+  <si>
+    <t>Automation note</t>
+  </si>
+  <si>
+    <t>noteText</t>
+  </si>
+  <si>
+    <t>verifyNotes</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunity</t>
+  </si>
+  <si>
+    <t>verifyOpportunities</t>
+  </si>
+  <si>
+    <t>verifyNewContract</t>
+  </si>
+  <si>
+    <t>verifyContracts</t>
+  </si>
+  <si>
+    <t>verifySearch</t>
+  </si>
+  <si>
+    <t>verifyHamburger</t>
+  </si>
+  <si>
+    <t>verifyDashboardHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyProfileIcon</t>
+  </si>
+  <si>
+    <t>verifyListingTypeOptions</t>
+  </si>
+  <si>
     <t>skip</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunityHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifySalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyLotsLabel</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,June,8,2020</t>
-  </si>
-  <si>
-    <t>salesType,branchName,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyAddSalesInformation</t>
-  </si>
-  <si>
-    <t>verifyAddVendorInfo</t>
-  </si>
-  <si>
-    <t>A Rigano Farms</t>
-  </si>
-  <si>
-    <t>vendorName</t>
-  </si>
-  <si>
-    <t>verifyAddLotsInfo</t>
-  </si>
-  <si>
-    <t>10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test</t>
-  </si>
-  <si>
-    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageHeaderLabels</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageValues</t>
-  </si>
-  <si>
-    <t>10,10,0</t>
-  </si>
-  <si>
-    <t>quantity,price,weight</t>
-  </si>
-  <si>
-    <t>verifyAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyAttachments</t>
-  </si>
-  <si>
-    <t>verifyAddNotes</t>
-  </si>
-  <si>
-    <t>Automation note</t>
-  </si>
-  <si>
-    <t>noteText</t>
-  </si>
-  <si>
-    <t>verifyNotes</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunity</t>
-  </si>
-  <si>
-    <t>verifyOpportunities</t>
-  </si>
-  <si>
-    <t>verifyNewContract</t>
-  </si>
-  <si>
-    <t>verifyContracts</t>
-  </si>
-  <si>
-    <t>verifySearch</t>
-  </si>
-  <si>
-    <t>verifyHamburger</t>
-  </si>
-  <si>
-    <t>verifyDashboardHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyProfileIcon</t>
-  </si>
-  <si>
-    <t>verifyListingTypeOptions</t>
   </si>
   <si>
     <t>verifyClassifiedListingType</t>
@@ -622,10 +622,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -678,7 +678,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,17 +701,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -723,16 +722,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -740,7 +738,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -761,14 +767,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -776,15 +774,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,6 +790,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -805,11 +805,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -822,7 +822,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,7 +888,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,163 +996,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,17 +1040,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1071,15 +1074,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1097,34 +1115,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1133,142 +1133,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1691,7 +1691,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="1"/>
@@ -1771,7 +1771,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="4">
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="10" ht="14.8" spans="1:2">
@@ -1874,7 +1874,7 @@
   <sheetPr/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1905,7 +1905,7 @@
         <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>79</v>
@@ -1919,7 +1919,7 @@
         <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>83</v>
@@ -1933,7 +1933,7 @@
         <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>86</v>
@@ -1947,7 +1947,7 @@
         <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>169</v>
@@ -1961,7 +1961,7 @@
         <v>171</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>172</v>
@@ -1975,7 +1975,7 @@
         <v>174</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
         <v>175</v>
@@ -1989,7 +1989,7 @@
         <v>177</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
         <v>178</v>
@@ -2003,7 +2003,7 @@
         <v>180</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2017,7 +2017,7 @@
         <v>182</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>183</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>184</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:3">
@@ -2041,7 +2041,7 @@
         <v>185</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>186</v>
@@ -2052,7 +2052,7 @@
         <v>187</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2165,7 +2165,6 @@
       <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8"/>
       <c r="D8" s="3"/>
     </row>
   </sheetData>
@@ -2180,7 +2179,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2235,7 +2234,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2263,183 +2262,183 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2453,8 +2452,8 @@
   <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2481,80 +2480,80 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -2570,8 +2569,8 @@
   <sheetPr/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2598,10 +2597,10 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2611,7 +2610,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2621,7 +2620,7 @@
         <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2631,7 +2630,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>79</v>
@@ -2645,7 +2644,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -2655,7 +2654,7 @@
         <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>83</v>
@@ -2669,7 +2668,7 @@
         <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>86</v>
@@ -2683,7 +2682,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>89</v>
@@ -2697,7 +2696,7 @@
         <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>92</v>
@@ -2711,7 +2710,7 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>95</v>
@@ -2725,7 +2724,7 @@
         <v>97</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -2735,7 +2734,7 @@
         <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>99</v>
@@ -2749,7 +2748,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
@@ -2796,7 +2795,7 @@
         <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>103</v>
@@ -2810,7 +2809,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>79</v>
@@ -2824,7 +2823,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2834,7 +2833,7 @@
         <v>107</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>108</v>
@@ -2848,7 +2847,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>111</v>
@@ -2862,7 +2861,7 @@
         <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>95</v>
@@ -2876,7 +2875,7 @@
         <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -2923,7 +2922,7 @@
         <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2933,7 +2932,7 @@
         <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2943,7 +2942,7 @@
         <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>118</v>
@@ -2994,7 +2993,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -3004,7 +3003,7 @@
         <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -3014,7 +3013,7 @@
         <v>122</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -3024,7 +3023,7 @@
         <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
@@ -3034,7 +3033,7 @@
         <v>124</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -3044,7 +3043,7 @@
         <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
@@ -3054,7 +3053,7 @@
         <v>126</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -3064,7 +3063,7 @@
         <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -3074,7 +3073,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
@@ -3084,7 +3083,7 @@
         <v>129</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
@@ -3094,7 +3093,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -3104,13 +3103,13 @@
         <v>131</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
@@ -3118,13 +3117,13 @@
         <v>132</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" ht="14.8" spans="1:4">
@@ -3132,7 +3131,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>134</v>
@@ -3146,7 +3145,7 @@
         <v>136</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>137</v>
@@ -3160,13 +3159,13 @@
         <v>139</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" ht="14.8" spans="1:4">
@@ -3174,7 +3173,7 @@
         <v>140</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
@@ -3184,7 +3183,7 @@
         <v>141</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
@@ -3194,7 +3193,7 @@
         <v>142</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
@@ -3204,13 +3203,13 @@
         <v>143</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" ht="14.8" spans="1:4">
@@ -3218,13 +3217,13 @@
         <v>144</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" ht="14.8" spans="1:4">
@@ -3232,7 +3231,7 @@
         <v>145</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>146</v>
@@ -3283,13 +3282,13 @@
         <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
@@ -3297,7 +3296,7 @@
         <v>150</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>151</v>
@@ -3311,7 +3310,7 @@
         <v>153</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3">
         <v>900</v>
@@ -3325,7 +3324,7 @@
         <v>155</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C5" s="5">
         <v>900</v>
@@ -3339,7 +3338,7 @@
         <v>157</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>158</v>
@@ -3353,7 +3352,7 @@
         <v>159</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -3363,7 +3362,7 @@
         <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>161</v>
@@ -3377,7 +3376,7 @@
         <v>163</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -3387,7 +3386,7 @@
         <v>164</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
fixed listing info sheep classified
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" activeTab="3"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198">
   <si>
     <t>Parameters</t>
   </si>
@@ -149,6 +149,9 @@
     <t>verifyNewOpportunityNavigation</t>
   </si>
   <si>
+    <t>skip</t>
+  </si>
+  <si>
     <t>verifyNewOpportunityHeaderLabel</t>
   </si>
   <si>
@@ -179,252 +182,252 @@
     <t>verifyAddVendorInfo</t>
   </si>
   <si>
+    <t>BR&amp;C Consignment Stock - GST</t>
+  </si>
+  <si>
+    <t>vendorName</t>
+  </si>
+  <si>
+    <t>verifyAddLotsInfo</t>
+  </si>
+  <si>
+    <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageHeaderLabels</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageValues</t>
+  </si>
+  <si>
+    <t>10,10,0</t>
+  </si>
+  <si>
+    <t>quantity,price,weight</t>
+  </si>
+  <si>
+    <t>verifyAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyAttachments</t>
+  </si>
+  <si>
+    <t>verifyAddNotes</t>
+  </si>
+  <si>
+    <t>Automation note</t>
+  </si>
+  <si>
+    <t>noteText</t>
+  </si>
+  <si>
+    <t>verifyNotes</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunity</t>
+  </si>
+  <si>
+    <t>verifyOpportunities</t>
+  </si>
+  <si>
+    <t>verifyNewContract</t>
+  </si>
+  <si>
+    <t>verifyContracts</t>
+  </si>
+  <si>
+    <t>verifySearch</t>
+  </si>
+  <si>
+    <t>verifyHamburger</t>
+  </si>
+  <si>
+    <t>verifyDashboardHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyProfileIcon</t>
+  </si>
+  <si>
+    <t>verifyListingTypeOptions</t>
+  </si>
+  <si>
+    <t>verifyClassifiedListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingType</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelection</t>
+  </si>
+  <si>
+    <t>Online,Dairy</t>
+  </si>
+  <si>
+    <t>transactionType,saleType</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigation</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
+  </si>
+  <si>
+    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetails</t>
+  </si>
+  <si>
+    <t>2,4,12,5,4,10</t>
+  </si>
+  <si>
+    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetails</t>
+  </si>
+  <si>
+    <t>Small,Prime,Test comment</t>
+  </si>
+  <si>
+    <t>frame,condition,agentComment</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetails</t>
+  </si>
+  <si>
+    <t>Yes,Quiet</t>
+  </si>
+  <si>
+    <t>vendorBred,temperament</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetails</t>
+  </si>
+  <si>
+    <t>Yes,Yes</t>
+  </si>
+  <si>
+    <t>hgpTreated,withinWithholdingPeriod</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingLiveWeightDetails</t>
+  </si>
+  <si>
+    <t>20,Fat score 1 (0-2mm)</t>
+  </si>
+  <si>
+    <t>liveWeight,fatScore</t>
+  </si>
+  <si>
+    <t>verifyPublishListing</t>
+  </si>
+  <si>
+    <t>CreateOpportunityForClassified</t>
+  </si>
+  <si>
+    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
+  </si>
+  <si>
+    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelectionClassified</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigationClassified</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>14 days,150,Test Description</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetails</t>
+  </si>
+  <si>
+    <t>Polled,10,20</t>
+  </si>
+  <si>
+    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListing</t>
+  </si>
+  <si>
+    <t>verifyOpportunityIdNavigationFromGridPage</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigationFromListingPage</t>
+  </si>
+  <si>
+    <t>verifyFillingNewContract</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
+  </si>
+  <si>
+    <t>salesType,branchName,buyerName,deliveryPoint</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewContractHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractSalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyBuyerInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyDeliveryInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyAdditionalChargesLabel</t>
+  </si>
+  <si>
+    <t>verifyCommissionAndAgentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddVendorInfo</t>
+  </si>
+  <si>
     <t>A Rigano Farms</t>
   </si>
   <si>
-    <t>vendorName</t>
-  </si>
-  <si>
-    <t>verifyAddLotsInfo</t>
-  </si>
-  <si>
-    <t>10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test</t>
-  </si>
-  <si>
-    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageHeaderLabels</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageValues</t>
-  </si>
-  <si>
-    <t>10,10,0</t>
-  </si>
-  <si>
-    <t>quantity,price,weight</t>
-  </si>
-  <si>
-    <t>verifyAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyAttachments</t>
-  </si>
-  <si>
-    <t>verifyAddNotes</t>
-  </si>
-  <si>
-    <t>Automation note</t>
-  </si>
-  <si>
-    <t>noteText</t>
-  </si>
-  <si>
-    <t>verifyNotes</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunity</t>
-  </si>
-  <si>
-    <t>verifyOpportunities</t>
-  </si>
-  <si>
-    <t>verifyNewContract</t>
-  </si>
-  <si>
-    <t>verifyContracts</t>
-  </si>
-  <si>
-    <t>verifySearch</t>
-  </si>
-  <si>
-    <t>verifyHamburger</t>
-  </si>
-  <si>
-    <t>verifyDashboardHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyProfileIcon</t>
-  </si>
-  <si>
-    <t>verifyListingTypeOptions</t>
-  </si>
-  <si>
-    <t>skip</t>
-  </si>
-  <si>
-    <t>verifyClassifiedListingType</t>
-  </si>
-  <si>
-    <t>verifyBidAndOfferListingType</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelection</t>
-  </si>
-  <si>
-    <t>Online,Dairy</t>
-  </si>
-  <si>
-    <t>transactionType,saleType</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigation</t>
-  </si>
-  <si>
-    <t>verifyFillingListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
-  </si>
-  <si>
-    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
-  </si>
-  <si>
-    <t>verifyFillingWeightsSummaryDetails</t>
-  </si>
-  <si>
-    <t>2,4,12,5,4,10</t>
-  </si>
-  <si>
-    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
-  </si>
-  <si>
-    <t>verifyFillingAssessmentOverviewDetails</t>
-  </si>
-  <si>
-    <t>Small,Prime,Test comment</t>
-  </si>
-  <si>
-    <t>frame,condition,agentComment</t>
-  </si>
-  <si>
-    <t>verifyFillingBreedingOverviewDetails</t>
-  </si>
-  <si>
-    <t>Yes,Quiet</t>
-  </si>
-  <si>
-    <t>vendorBred,temperament</t>
-  </si>
-  <si>
-    <t>verifyFillingHealthVetDetails</t>
-  </si>
-  <si>
-    <t>Yes,Yes</t>
-  </si>
-  <si>
-    <t>hgpTreated,withinWithholdingPeriod</t>
-  </si>
-  <si>
-    <t>verifyFillingDeliveryDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingLiveWeightDetails</t>
-  </si>
-  <si>
-    <t>20,Fat score 1 (0-2mm)</t>
-  </si>
-  <si>
-    <t>liveWeight,fatScore</t>
-  </si>
-  <si>
-    <t>verifyPublishListing</t>
-  </si>
-  <si>
-    <t>CreateOpportunityForClassified</t>
-  </si>
-  <si>
-    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
-  </si>
-  <si>
-    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelectionClassified</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigationClassified</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>14 days,150,Test Description</t>
-  </si>
-  <si>
-    <t>classifiedDuration,price,description</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedLotDetails</t>
-  </si>
-  <si>
-    <t>Polled,10,20</t>
-  </si>
-  <si>
-    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedHealthVetDetails</t>
-  </si>
-  <si>
-    <t>verifyClassifiedPublishListing</t>
-  </si>
-  <si>
-    <t>verifyOpportunityIdNavigationFromGridPage</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigationFromListingPage</t>
-  </si>
-  <si>
-    <t>verifyFillingNewContract</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
-  </si>
-  <si>
-    <t>salesType,branchName,buyerName,deliveryPoint</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigation</t>
-  </si>
-  <si>
-    <t>verifyNewContractHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractSalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyBuyerInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyDeliveryInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractLotsLabel</t>
-  </si>
-  <si>
-    <t>verifyAdditionalChargesLabel</t>
-  </si>
-  <si>
-    <t>verifyCommissionAndAgentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddSalesInformation</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddVendorInfo</t>
-  </si>
-  <si>
     <t>verifyAddBuyerInfo</t>
   </si>
   <si>
@@ -599,7 +602,7 @@
     <t>verifyFillingClassifiedListingOverviewDetailsSheep</t>
   </si>
   <si>
-    <t>14 days,150,Test Description,BEULAH</t>
+    <t>14 days,150,Test Description,AARONS</t>
   </si>
   <si>
     <t>classifiedDuration,price,description,town</t>
@@ -622,10 +625,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -671,37 +674,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -709,36 +682,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -760,8 +703,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,9 +756,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -791,17 +794,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -812,6 +808,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -819,12 +822,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -840,7 +837,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,13 +891,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,7 +933,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,19 +957,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -906,103 +1005,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,63 +1030,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1114,6 +1060,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1128,150 +1098,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1902,10 +1905,10 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>79</v>
@@ -1916,10 +1919,10 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>83</v>
@@ -1930,10 +1933,10 @@
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>86</v>
@@ -1944,115 +1947,115 @@
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2067,7 +2070,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>37</v>
@@ -2104,7 +2107,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -2114,21 +2117,21 @@
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>37</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>37</v>
@@ -2152,7 +2155,7 @@
     </row>
     <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>37</v>
@@ -2160,7 +2163,7 @@
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>37</v>
@@ -2234,7 +2237,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2262,183 +2265,183 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2452,8 +2455,8 @@
   <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2480,80 +2483,80 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -2597,10 +2600,10 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2610,7 +2613,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2620,7 +2623,7 @@
         <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2630,7 +2633,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>79</v>
@@ -2644,7 +2647,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -2654,7 +2657,7 @@
         <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>83</v>
@@ -2668,7 +2671,7 @@
         <v>85</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>86</v>
@@ -2682,7 +2685,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>89</v>
@@ -2696,7 +2699,7 @@
         <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>92</v>
@@ -2710,7 +2713,7 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>95</v>
@@ -2724,7 +2727,7 @@
         <v>97</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -2734,7 +2737,7 @@
         <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>99</v>
@@ -2748,7 +2751,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
@@ -2764,8 +2767,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2795,7 +2798,7 @@
         <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>103</v>
@@ -2809,7 +2812,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>79</v>
@@ -2823,7 +2826,7 @@
         <v>106</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2833,7 +2836,7 @@
         <v>107</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>108</v>
@@ -2847,7 +2850,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>111</v>
@@ -2861,7 +2864,7 @@
         <v>113</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>95</v>
@@ -2875,7 +2878,7 @@
         <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -2922,7 +2925,7 @@
         <v>115</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2932,7 +2935,7 @@
         <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2942,7 +2945,7 @@
         <v>117</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>118</v>
@@ -2962,8 +2965,8 @@
   <sheetPr/>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2993,7 +2996,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -3003,7 +3006,7 @@
         <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -3013,7 +3016,7 @@
         <v>122</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -3023,7 +3026,7 @@
         <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
@@ -3033,7 +3036,7 @@
         <v>124</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -3043,7 +3046,7 @@
         <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
@@ -3053,7 +3056,7 @@
         <v>126</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -3063,7 +3066,7 @@
         <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -3073,7 +3076,7 @@
         <v>128</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
@@ -3083,7 +3086,7 @@
         <v>129</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
@@ -3093,7 +3096,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -3103,13 +3106,13 @@
         <v>131</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
@@ -3117,127 +3120,127 @@
         <v>132</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" ht="14.8" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" ht="14.8" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" ht="14.8" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" ht="14.8" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" ht="14.8" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" ht="14.8" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3279,114 +3282,114 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3">
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5">
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
completed E-contract from dashboard test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="3" activeTab="7"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200">
   <si>
     <t>Parameters</t>
   </si>
@@ -422,6 +422,9 @@
     <t>verifyNewContractAddSalesInformation</t>
   </si>
   <si>
+    <t>Dairy,ALBANY,June,8,2020</t>
+  </si>
+  <si>
     <t>verifyNewContractAddVendorInfo</t>
   </si>
   <si>
@@ -455,6 +458,9 @@
     <t>verifyAddCommissionAndAgents</t>
   </si>
   <si>
+    <t>verifyNewContractAddAttachments</t>
+  </si>
+  <si>
     <t>verifyNewContractAttachments</t>
   </si>
   <si>
@@ -467,10 +473,10 @@
     <t>verifyValidateContract</t>
   </si>
   <si>
-    <t>Ashish</t>
-  </si>
-  <si>
-    <t>signatureText</t>
+    <t>Ashish,Test Buyer,Test Vendor</t>
+  </si>
+  <si>
+    <t>agentSignature,buyerSignature,VendorSignature</t>
   </si>
   <si>
     <t>VerifyAddingSalesAndVendorInfo</t>
@@ -665,41 +671,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -719,6 +718,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -727,23 +755,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -756,8 +792,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -779,38 +816,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -825,25 +831,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,61 +855,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,13 +891,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -945,67 +1011,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,27 +1040,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1070,16 +1059,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1100,16 +1089,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1122,162 +1137,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1905,7 +1911,7 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
@@ -1919,7 +1925,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
@@ -1933,7 +1939,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -1947,63 +1953,63 @@
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -2012,12 +2018,12 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>
@@ -2025,7 +2031,7 @@
     </row>
     <row r="11" ht="15.75" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>41</v>
@@ -2033,7 +2039,7 @@
     </row>
     <row r="12" ht="15.75" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>41</v>
@@ -2041,18 +2047,18 @@
     </row>
     <row r="13" ht="15.75" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>41</v>
@@ -2070,7 +2076,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2097,44 +2103,44 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>111</v>
@@ -2145,28 +2151,28 @@
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -2963,10 +2969,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -3109,7 +3115,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>47</v>
@@ -3117,13 +3123,13 @@
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>53</v>
@@ -3131,35 +3137,35 @@
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
@@ -3173,7 +3179,7 @@
     </row>
     <row r="18" ht="14.8" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>37</v>
@@ -3183,7 +3189,7 @@
     </row>
     <row r="19" ht="14.8" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>37</v>
@@ -3193,7 +3199,7 @@
     </row>
     <row r="20" ht="14.8" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>37</v>
@@ -3203,21 +3209,17 @@
     </row>
     <row r="21" ht="14.8" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" ht="14.8" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>37</v>
@@ -3231,16 +3233,30 @@
     </row>
     <row r="23" ht="14.8" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>147</v>
+        <v>64</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" ht="14.8" spans="1:4">
+      <c r="A24" s="4" t="s">
         <v>148</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3282,13 +3298,13 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>53</v>
@@ -3296,21 +3312,21 @@
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
@@ -3319,12 +3335,12 @@
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>41</v>
@@ -3333,26 +3349,26 @@
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>41</v>
@@ -3362,21 +3378,21 @@
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>41</v>
@@ -3386,7 +3402,7 @@
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
fixed e-contract test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -428,13 +428,13 @@
     <t>verifyNewContractAddVendorInfo</t>
   </si>
   <si>
-    <t>A Rigano Farms</t>
+    <t>Corrigin Cash account</t>
   </si>
   <si>
     <t>verifyAddBuyerInfo</t>
   </si>
   <si>
-    <t>AJ Pointon &amp; AW Pointon</t>
+    <t>Chatley &amp; Hutcheson</t>
   </si>
   <si>
     <t>buyerName</t>
@@ -631,10 +631,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -671,6 +671,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -679,23 +701,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -719,13 +726,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -739,9 +739,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -770,28 +769,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -801,7 +778,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -816,7 +816,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -831,7 +831,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,13 +879,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,7 +903,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,25 +987,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,115 +1011,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,6 +1059,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1069,36 +1084,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1129,6 +1114,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1142,148 +1142,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2972,7 +2972,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
fixed e-contract test cases and listing info test cases as well
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="7" activeTab="7"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201">
   <si>
     <t>Parameters</t>
   </si>
@@ -149,307 +149,310 @@
     <t>verifyNewOpportunityNavigation</t>
   </si>
   <si>
+    <t>verifyNewOpportunityHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifySalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyAddSalesInformation</t>
+  </si>
+  <si>
+    <t>verifyAddVendorInfo</t>
+  </si>
+  <si>
+    <t>BR&amp;C Consignment Stock - GST</t>
+  </si>
+  <si>
+    <t>vendorName</t>
+  </si>
+  <si>
+    <t>verifyAddLotsInfo</t>
+  </si>
+  <si>
+    <t>10,Cattle,Bull,Angus,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageHeaderLabels</t>
+  </si>
+  <si>
+    <t>verifyLotSummaryPageValues</t>
+  </si>
+  <si>
+    <t>10,10,0</t>
+  </si>
+  <si>
+    <t>quantity,price,weight</t>
+  </si>
+  <si>
+    <t>verifyAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyAttachments</t>
+  </si>
+  <si>
+    <t>verifyAddNotes</t>
+  </si>
+  <si>
+    <t>Automation note</t>
+  </si>
+  <si>
+    <t>noteText</t>
+  </si>
+  <si>
+    <t>verifyNotes</t>
+  </si>
+  <si>
+    <t>verifyNewOpportunity</t>
+  </si>
+  <si>
     <t>skip</t>
   </si>
   <si>
-    <t>verifyNewOpportunityHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifySalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyLotsLabel</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,June,8,2020</t>
+    <t>verifyOpportunities</t>
+  </si>
+  <si>
+    <t>verifyNewContract</t>
+  </si>
+  <si>
+    <t>verifyContracts</t>
+  </si>
+  <si>
+    <t>verifySearch</t>
+  </si>
+  <si>
+    <t>verifyHamburger</t>
+  </si>
+  <si>
+    <t>verifyDashboardHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyProfileIcon</t>
+  </si>
+  <si>
+    <t>verifyListingTypeOptions</t>
+  </si>
+  <si>
+    <t>verifyClassifiedListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingType</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelection</t>
+  </si>
+  <si>
+    <t>Online,Store</t>
+  </si>
+  <si>
+    <t>transactionType,saleType</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigation</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
+  </si>
+  <si>
+    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetails</t>
+  </si>
+  <si>
+    <t>2,4,12,5,4,10</t>
+  </si>
+  <si>
+    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetails</t>
+  </si>
+  <si>
+    <t>Small,Prime,Test comment</t>
+  </si>
+  <si>
+    <t>frame,condition,agentComment</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetails</t>
+  </si>
+  <si>
+    <t>Yes,Quiet</t>
+  </si>
+  <si>
+    <t>vendorBred,temperament</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetails</t>
+  </si>
+  <si>
+    <t>Yes,Yes</t>
+  </si>
+  <si>
+    <t>hgpTreated,withinWithholdingPeriod</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingLiveWeightDetails</t>
+  </si>
+  <si>
+    <t>20,Fat score 1 (0-2mm)</t>
+  </si>
+  <si>
+    <t>liveWeight,fatScore</t>
+  </si>
+  <si>
+    <t>verifyPublishListing</t>
+  </si>
+  <si>
+    <t>CreateOpportunityForClassified</t>
+  </si>
+  <si>
+    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
+  </si>
+  <si>
+    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelectionClassified</t>
+  </si>
+  <si>
+    <t>Online,Dairy</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigationClassified</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>14 days,150,Test Description</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetails</t>
+  </si>
+  <si>
+    <t>Polled,10,20</t>
+  </si>
+  <si>
+    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListing</t>
+  </si>
+  <si>
+    <t>verifyOpportunityIdNavigationFromGridPage</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigationFromListingPage</t>
+  </si>
+  <si>
+    <t>verifyFillingNewContract</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
+  </si>
+  <si>
+    <t>salesType,branchName,buyerName,deliveryPoint</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewContractHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractSalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyBuyerInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyDeliveryInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyAdditionalChargesLabel</t>
+  </si>
+  <si>
+    <t>verifyCommissionAndAgentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddSalesInformation</t>
+  </si>
+  <si>
+    <t>Dairy,ALBANY,June,8,2020</t>
   </si>
   <si>
     <t>salesType,branchName,month,day,year</t>
   </si>
   <si>
-    <t>verifyNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyAddSalesInformation</t>
-  </si>
-  <si>
-    <t>verifyAddVendorInfo</t>
-  </si>
-  <si>
-    <t>BR&amp;C Consignment Stock - GST</t>
-  </si>
-  <si>
-    <t>vendorName</t>
-  </si>
-  <si>
-    <t>verifyAddLotsInfo</t>
+    <t>verifyNewContractAddVendorInfo</t>
+  </si>
+  <si>
+    <t>Corrigin Cash account</t>
+  </si>
+  <si>
+    <t>verifyAddBuyerInfo</t>
+  </si>
+  <si>
+    <t>Chatley &amp; Hutcheson</t>
+  </si>
+  <si>
+    <t>buyerName</t>
+  </si>
+  <si>
+    <t>verifyAddDeliveryInfo</t>
+  </si>
+  <si>
+    <t>Test Delivery Point,June,12,2020</t>
+  </si>
+  <si>
+    <t>deliveryPoint,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddLotsInfo</t>
   </si>
   <si>
     <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
-  </si>
-  <si>
-    <t>quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageHeaderLabels</t>
-  </si>
-  <si>
-    <t>verifyLotSummaryPageValues</t>
-  </si>
-  <si>
-    <t>10,10,0</t>
-  </si>
-  <si>
-    <t>quantity,price,weight</t>
-  </si>
-  <si>
-    <t>verifyAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyAttachments</t>
-  </si>
-  <si>
-    <t>verifyAddNotes</t>
-  </si>
-  <si>
-    <t>Automation note</t>
-  </si>
-  <si>
-    <t>noteText</t>
-  </si>
-  <si>
-    <t>verifyNotes</t>
-  </si>
-  <si>
-    <t>verifyNewOpportunity</t>
-  </si>
-  <si>
-    <t>verifyOpportunities</t>
-  </si>
-  <si>
-    <t>verifyNewContract</t>
-  </si>
-  <si>
-    <t>verifyContracts</t>
-  </si>
-  <si>
-    <t>verifySearch</t>
-  </si>
-  <si>
-    <t>verifyHamburger</t>
-  </si>
-  <si>
-    <t>verifyDashboardHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyProfileIcon</t>
-  </si>
-  <si>
-    <t>verifyListingTypeOptions</t>
-  </si>
-  <si>
-    <t>verifyClassifiedListingType</t>
-  </si>
-  <si>
-    <t>verifyBidAndOfferListingType</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelection</t>
-  </si>
-  <si>
-    <t>Online,Dairy</t>
-  </si>
-  <si>
-    <t>transactionType,saleType</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigation</t>
-  </si>
-  <si>
-    <t>verifyFillingListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
-  </si>
-  <si>
-    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
-  </si>
-  <si>
-    <t>verifyFillingWeightsSummaryDetails</t>
-  </si>
-  <si>
-    <t>2,4,12,5,4,10</t>
-  </si>
-  <si>
-    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
-  </si>
-  <si>
-    <t>verifyFillingAssessmentOverviewDetails</t>
-  </si>
-  <si>
-    <t>Small,Prime,Test comment</t>
-  </si>
-  <si>
-    <t>frame,condition,agentComment</t>
-  </si>
-  <si>
-    <t>verifyFillingBreedingOverviewDetails</t>
-  </si>
-  <si>
-    <t>Yes,Quiet</t>
-  </si>
-  <si>
-    <t>vendorBred,temperament</t>
-  </si>
-  <si>
-    <t>verifyFillingHealthVetDetails</t>
-  </si>
-  <si>
-    <t>Yes,Yes</t>
-  </si>
-  <si>
-    <t>hgpTreated,withinWithholdingPeriod</t>
-  </si>
-  <si>
-    <t>verifyFillingDeliveryDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingLiveWeightDetails</t>
-  </si>
-  <si>
-    <t>20,Fat score 1 (0-2mm)</t>
-  </si>
-  <si>
-    <t>liveWeight,fatScore</t>
-  </si>
-  <si>
-    <t>verifyPublishListing</t>
-  </si>
-  <si>
-    <t>CreateOpportunityForClassified</t>
-  </si>
-  <si>
-    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
-  </si>
-  <si>
-    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelectionClassified</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigationClassified</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>14 days,150,Test Description</t>
-  </si>
-  <si>
-    <t>classifiedDuration,price,description</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedLotDetails</t>
-  </si>
-  <si>
-    <t>Polled,10,20</t>
-  </si>
-  <si>
-    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedHealthVetDetails</t>
-  </si>
-  <si>
-    <t>verifyClassifiedPublishListing</t>
-  </si>
-  <si>
-    <t>verifyOpportunityIdNavigationFromGridPage</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigationFromListingPage</t>
-  </si>
-  <si>
-    <t>verifyFillingNewContract</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
-  </si>
-  <si>
-    <t>salesType,branchName,buyerName,deliveryPoint</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigation</t>
-  </si>
-  <si>
-    <t>verifyNewContractHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractSalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyBuyerInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyDeliveryInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractLotsLabel</t>
-  </si>
-  <si>
-    <t>verifyAdditionalChargesLabel</t>
-  </si>
-  <si>
-    <t>verifyCommissionAndAgentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddSalesInformation</t>
-  </si>
-  <si>
-    <t>Dairy,ALBANY,June,8,2020</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddVendorInfo</t>
-  </si>
-  <si>
-    <t>Corrigin Cash account</t>
-  </si>
-  <si>
-    <t>verifyAddBuyerInfo</t>
-  </si>
-  <si>
-    <t>Chatley &amp; Hutcheson</t>
-  </si>
-  <si>
-    <t>buyerName</t>
-  </si>
-  <si>
-    <t>verifyAddDeliveryInfo</t>
-  </si>
-  <si>
-    <t>Test Delivery Point,June,12,2020</t>
-  </si>
-  <si>
-    <t>deliveryPoint,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddLotsInfo</t>
   </si>
   <si>
     <t>verifyAddAdditionalCharges</t>
@@ -632,9 +635,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -686,32 +689,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,21 +727,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,16 +741,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -778,7 +788,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,33 +802,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -831,7 +834,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,49 +900,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,7 +924,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,13 +966,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,43 +1002,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -975,43 +1014,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,15 +1039,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1088,6 +1082,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1114,17 +1123,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1142,142 +1145,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1911,157 +1914,157 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2103,76 +2106,76 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -2243,7 +2246,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2271,183 +2274,179 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2489,80 +2488,80 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -2578,8 +2577,8 @@
   <sheetPr/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2606,158 +2605,158 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="3"/>
@@ -2801,90 +2800,90 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -2928,36 +2927,36 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2971,8 +2970,8 @@
   <sheetPr/>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2999,126 +2998,126 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
@@ -3126,13 +3125,13 @@
         <v>133</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>134</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" ht="14.8" spans="1:4">
@@ -3140,7 +3139,7 @@
         <v>135</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>136</v>
@@ -3154,7 +3153,7 @@
         <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>139</v>
@@ -3168,95 +3167,95 @@
         <v>141</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" ht="14.8" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" ht="14.8" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" ht="14.8" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" ht="14.8" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" ht="14.8" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" ht="14.8" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" ht="14.8" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3298,114 +3297,114 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3">
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5">
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
fixed listing info issues
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205">
   <si>
     <t>Parameters</t>
   </si>
@@ -269,274 +269,286 @@
     <t>verifyFillingListingOverviewDetails</t>
   </si>
   <si>
+    <t>24 hours,3 hours,200,Test Description,215,AARONS</t>
+  </si>
+  <si>
+    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
+  </si>
+  <si>
+    <t>verifyFillingWeightsSummaryDetails</t>
+  </si>
+  <si>
+    <t>2,4,12,5,4,10</t>
+  </si>
+  <si>
+    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
+  </si>
+  <si>
+    <t>verifyFillingAssessmentOverviewDetails</t>
+  </si>
+  <si>
+    <t>Small,Prime,Test comment</t>
+  </si>
+  <si>
+    <t>frame,condition,agentComment</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingOverviewDetails</t>
+  </si>
+  <si>
+    <t>Yes,Quiet</t>
+  </si>
+  <si>
+    <t>vendorBred,temperament</t>
+  </si>
+  <si>
+    <t>verifyFillingHealthVetDetails</t>
+  </si>
+  <si>
+    <t>Yes,Yes</t>
+  </si>
+  <si>
+    <t>hgpTreated,withinWithholdingPeriod</t>
+  </si>
+  <si>
+    <t>verifyFillingDeliveryDetails</t>
+  </si>
+  <si>
+    <t>verifyFillingLiveWeightDetails</t>
+  </si>
+  <si>
+    <t>20,Fat score 1 (0-2mm)</t>
+  </si>
+  <si>
+    <t>liveWeight,fatScore</t>
+  </si>
+  <si>
+    <t>verifyFillingBreedingDetails</t>
+  </si>
+  <si>
+    <t>Test Sire,Test Dam,10</t>
+  </si>
+  <si>
+    <t>sire,dam,noOfHead</t>
+  </si>
+  <si>
+    <t>verifyPublishListing</t>
+  </si>
+  <si>
+    <t>CreateOpportunityForClassified</t>
+  </si>
+  <si>
+    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
+  </si>
+  <si>
+    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
+  </si>
+  <si>
+    <t>verifyListingTypeSelectionClassified</t>
+  </si>
+  <si>
+    <t>Online,Dairy</t>
+  </si>
+  <si>
+    <t>verifyListingInfoNavigationClassified</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>14 days,150,Test Description</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetails</t>
+  </si>
+  <si>
+    <t>Polled,10,20</t>
+  </si>
+  <si>
+    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListing</t>
+  </si>
+  <si>
+    <t>verifyOpportunityIdNavigationFromGridPage</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigationFromListingPage</t>
+  </si>
+  <si>
+    <t>verifyFillingNewContract</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
+  </si>
+  <si>
+    <t>salesType,branchName,buyerName,deliveryPoint</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewContractHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractSalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyBuyerInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyDeliveryInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyAdditionalChargesLabel</t>
+  </si>
+  <si>
+    <t>verifyCommissionAndAgentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddSalesInformation</t>
+  </si>
+  <si>
+    <t>Dairy,ALBANY,June,8,2020</t>
+  </si>
+  <si>
+    <t>salesType,branchName,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddVendorInfo</t>
+  </si>
+  <si>
+    <t>Corrigin Cash account</t>
+  </si>
+  <si>
+    <t>verifyAddBuyerInfo</t>
+  </si>
+  <si>
+    <t>Chatley &amp; Hutcheson</t>
+  </si>
+  <si>
+    <t>buyerName</t>
+  </si>
+  <si>
+    <t>verifyAddDeliveryInfo</t>
+  </si>
+  <si>
+    <t>Test Delivery Point,June,12,2020</t>
+  </si>
+  <si>
+    <t>deliveryPoint,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddLotsInfo</t>
+  </si>
+  <si>
+    <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>verifyAddAdditionalCharges</t>
+  </si>
+  <si>
+    <t>verifyAddCommissionAndAgents</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachments</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddNotes</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotes</t>
+  </si>
+  <si>
+    <t>verifyValidateContract</t>
+  </si>
+  <si>
+    <t>Ashish,Test Buyer,Test Vendor</t>
+  </si>
+  <si>
+    <t>agentSignature,buyerSignature,VendorSignature</t>
+  </si>
+  <si>
+    <t>VerifyAddingSalesAndVendorInfo</t>
+  </si>
+  <si>
+    <t>A Rigano</t>
+  </si>
+  <si>
+    <t>verifyPerKGConditionInLot</t>
+  </si>
+  <si>
+    <t>15,Sheep,Ewe,Bond</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed</t>
+  </si>
+  <si>
+    <t>verifyAddingValueToPerKGFieldInLot</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>verifyWeightValueOnLotGridPage</t>
+  </si>
+  <si>
+    <t>quantity,weight</t>
+  </si>
+  <si>
+    <t>verifyAddingSecondLotInTheSameOpportunity</t>
+  </si>
+  <si>
+    <t>10,Cattle,Buffalo,Angus</t>
+  </si>
+  <si>
+    <t>verifyDisabledListingType</t>
+  </si>
+  <si>
+    <t>VerifyEditingLotsInfo</t>
+  </si>
+  <si>
+    <t>Cheviot</t>
+  </si>
+  <si>
+    <t>updatedBreed</t>
+  </si>
+  <si>
+    <t>VerifyDeletingLot</t>
+  </si>
+  <si>
+    <t>verifyEnabledListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingTypeSelection</t>
+  </si>
+  <si>
+    <t>verifyFillingListingOverviewDetailsForSheep</t>
+  </si>
+  <si>
     <t>24 hours,3 hours,200,Test Description,215,BEULAH</t>
-  </si>
-  <si>
-    <t>biddingDuration,closingSoonStatusDuration,startingPrice,description,reservePrice,town</t>
-  </si>
-  <si>
-    <t>verifyFillingWeightsSummaryDetails</t>
-  </si>
-  <si>
-    <t>2,4,12,5,4,10</t>
-  </si>
-  <si>
-    <t>numberOfHeadWeighted,hoursOffFeed,estimatedDressing,estimatedDaysToDelivery,estimatedWeightGain,deliveryAdjustment</t>
-  </si>
-  <si>
-    <t>verifyFillingAssessmentOverviewDetails</t>
-  </si>
-  <si>
-    <t>Small,Prime,Test comment</t>
-  </si>
-  <si>
-    <t>frame,condition,agentComment</t>
-  </si>
-  <si>
-    <t>verifyFillingBreedingOverviewDetails</t>
-  </si>
-  <si>
-    <t>Yes,Quiet</t>
-  </si>
-  <si>
-    <t>vendorBred,temperament</t>
-  </si>
-  <si>
-    <t>verifyFillingHealthVetDetails</t>
-  </si>
-  <si>
-    <t>Yes,Yes</t>
-  </si>
-  <si>
-    <t>hgpTreated,withinWithholdingPeriod</t>
-  </si>
-  <si>
-    <t>verifyFillingDeliveryDetails</t>
-  </si>
-  <si>
-    <t>verifyFillingLiveWeightDetails</t>
-  </si>
-  <si>
-    <t>20,Fat score 1 (0-2mm)</t>
-  </si>
-  <si>
-    <t>liveWeight,fatScore</t>
-  </si>
-  <si>
-    <t>verifyPublishListing</t>
-  </si>
-  <si>
-    <t>CreateOpportunityForClassified</t>
-  </si>
-  <si>
-    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
-  </si>
-  <si>
-    <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
-  </si>
-  <si>
-    <t>verifyListingTypeSelectionClassified</t>
-  </si>
-  <si>
-    <t>Online,Dairy</t>
-  </si>
-  <si>
-    <t>verifyListingInfoNavigationClassified</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>14 days,150,Test Description</t>
-  </si>
-  <si>
-    <t>classifiedDuration,price,description</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedLotDetails</t>
-  </si>
-  <si>
-    <t>Polled,10,20</t>
-  </si>
-  <si>
-    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedHealthVetDetails</t>
-  </si>
-  <si>
-    <t>verifyClassifiedPublishListing</t>
-  </si>
-  <si>
-    <t>verifyOpportunityIdNavigationFromGridPage</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigationFromListingPage</t>
-  </si>
-  <si>
-    <t>verifyFillingNewContract</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
-  </si>
-  <si>
-    <t>salesType,branchName,buyerName,deliveryPoint</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigation</t>
-  </si>
-  <si>
-    <t>verifyNewContractHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractSalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyBuyerInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyDeliveryInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractLotsLabel</t>
-  </si>
-  <si>
-    <t>verifyAdditionalChargesLabel</t>
-  </si>
-  <si>
-    <t>verifyCommissionAndAgentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddSalesInformation</t>
-  </si>
-  <si>
-    <t>Dairy,ALBANY,June,8,2020</t>
-  </si>
-  <si>
-    <t>salesType,branchName,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddVendorInfo</t>
-  </si>
-  <si>
-    <t>Corrigin Cash account</t>
-  </si>
-  <si>
-    <t>verifyAddBuyerInfo</t>
-  </si>
-  <si>
-    <t>Chatley &amp; Hutcheson</t>
-  </si>
-  <si>
-    <t>buyerName</t>
-  </si>
-  <si>
-    <t>verifyAddDeliveryInfo</t>
-  </si>
-  <si>
-    <t>Test Delivery Point,June,12,2020</t>
-  </si>
-  <si>
-    <t>deliveryPoint,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddLotsInfo</t>
-  </si>
-  <si>
-    <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
-  </si>
-  <si>
-    <t>verifyAddAdditionalCharges</t>
-  </si>
-  <si>
-    <t>verifyAddCommissionAndAgents</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachments</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddNotes</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotes</t>
-  </si>
-  <si>
-    <t>verifyValidateContract</t>
-  </si>
-  <si>
-    <t>Ashish,Test Buyer,Test Vendor</t>
-  </si>
-  <si>
-    <t>agentSignature,buyerSignature,VendorSignature</t>
-  </si>
-  <si>
-    <t>VerifyAddingSalesAndVendorInfo</t>
-  </si>
-  <si>
-    <t>A Rigano</t>
-  </si>
-  <si>
-    <t>verifyPerKGConditionInLot</t>
-  </si>
-  <si>
-    <t>15,Sheep,Ewe,Bond</t>
-  </si>
-  <si>
-    <t>quantity,productCategory,product,breed</t>
-  </si>
-  <si>
-    <t>verifyAddingValueToPerKGFieldInLot</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>verifyWeightValueOnLotGridPage</t>
-  </si>
-  <si>
-    <t>quantity,weight</t>
-  </si>
-  <si>
-    <t>verifyAddingSecondLotInTheSameOpportunity</t>
-  </si>
-  <si>
-    <t>10,Cattle,Buffalo,Angus</t>
-  </si>
-  <si>
-    <t>verifyDisabledListingType</t>
-  </si>
-  <si>
-    <t>VerifyEditingLotsInfo</t>
-  </si>
-  <si>
-    <t>Cheviot</t>
-  </si>
-  <si>
-    <t>updatedBreed</t>
-  </si>
-  <si>
-    <t>VerifyDeletingLot</t>
-  </si>
-  <si>
-    <t>verifyEnabledListingType</t>
-  </si>
-  <si>
-    <t>verifyBidAndOfferListingTypeSelection</t>
-  </si>
-  <si>
-    <t>verifyFillingListingOverviewDetailsForSheep</t>
   </si>
   <si>
     <t>verifyFillingWeightsSummaryDetailsForSheep</t>
@@ -634,10 +646,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -689,28 +701,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -733,16 +723,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -756,8 +746,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -779,14 +792,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -795,7 +800,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -809,19 +814,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -834,7 +846,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,13 +870,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -864,7 +894,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,7 +912,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,127 +1026,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,6 +1060,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1108,6 +1129,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1122,165 +1152,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1914,13 +1926,13 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
@@ -1928,13 +1940,13 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>174</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>82</v>
@@ -1942,7 +1954,7 @@
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
@@ -1956,63 +1968,63 @@
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -2021,12 +2033,12 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>
@@ -2034,7 +2046,7 @@
     </row>
     <row r="11" ht="15.75" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -2042,7 +2054,7 @@
     </row>
     <row r="12" ht="15.75" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
@@ -2050,18 +2062,18 @@
     </row>
     <row r="13" ht="15.75" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>65</v>
@@ -2106,7 +2118,7 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
@@ -2116,7 +2128,7 @@
     </row>
     <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
@@ -2126,35 +2138,35 @@
     </row>
     <row r="4" ht="15.75" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
@@ -2164,7 +2176,7 @@
     </row>
     <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
@@ -2172,7 +2184,7 @@
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
@@ -2575,10 +2587,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2618,7 +2630,7 @@
         <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2758,8 +2770,22 @@
       <c r="B14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" ht="14.8" spans="1:4">
+      <c r="A15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2800,27 +2826,27 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>78</v>
@@ -2828,7 +2854,7 @@
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
@@ -2838,35 +2864,35 @@
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
@@ -2880,7 +2906,7 @@
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
@@ -2927,7 +2953,7 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
@@ -2937,7 +2963,7 @@
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
@@ -2947,16 +2973,16 @@
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2998,7 +3024,7 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
@@ -3008,7 +3034,7 @@
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
@@ -3018,7 +3044,7 @@
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
@@ -3028,7 +3054,7 @@
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
@@ -3038,7 +3064,7 @@
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
@@ -3048,7 +3074,7 @@
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
@@ -3058,7 +3084,7 @@
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
@@ -3068,7 +3094,7 @@
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -3078,7 +3104,7 @@
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>
@@ -3088,7 +3114,7 @@
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -3098,7 +3124,7 @@
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
@@ -3108,27 +3134,27 @@
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>50</v>
@@ -3136,41 +3162,41 @@
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>53</v>
@@ -3178,7 +3204,7 @@
     </row>
     <row r="18" ht="14.8" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -3188,7 +3214,7 @@
     </row>
     <row r="19" ht="14.8" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>65</v>
@@ -3198,7 +3224,7 @@
     </row>
     <row r="20" ht="14.8" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>65</v>
@@ -3208,7 +3234,7 @@
     </row>
     <row r="21" ht="14.8" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>65</v>
@@ -3218,7 +3244,7 @@
     </row>
     <row r="22" ht="14.8" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
@@ -3232,7 +3258,7 @@
     </row>
     <row r="23" ht="14.8" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -3246,16 +3272,16 @@
     </row>
     <row r="24" ht="14.8" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3297,13 +3323,13 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>50</v>
@@ -3311,21 +3337,21 @@
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
@@ -3334,12 +3360,12 @@
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
@@ -3348,26 +3374,26 @@
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
@@ -3377,21 +3403,21 @@
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -3401,7 +3427,7 @@
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
increased login time and introduced back space in classified listing info test case
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" activeTab="4"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -647,8 +647,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -708,31 +708,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -748,6 +726,37 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -770,30 +779,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -804,6 +790,21 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -823,15 +824,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -846,25 +846,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,13 +876,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,13 +978,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,115 +1026,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1059,15 +1059,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1088,17 +1079,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1118,37 +1138,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,142 +1157,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2091,7 +2091,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2589,8 +2589,8 @@
   <sheetPr/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2620,7 +2620,7 @@
         <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2640,7 +2640,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2650,7 +2650,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>77</v>
@@ -2664,7 +2664,7 @@
         <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -2674,7 +2674,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>81</v>
@@ -2688,7 +2688,7 @@
         <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>84</v>
@@ -2702,7 +2702,7 @@
         <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>87</v>
@@ -2716,7 +2716,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>90</v>
@@ -2730,7 +2730,7 @@
         <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>93</v>
@@ -2744,7 +2744,7 @@
         <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -2754,7 +2754,7 @@
         <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>97</v>
@@ -2768,7 +2768,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>100</v>
@@ -2782,7 +2782,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
@@ -2799,7 +2799,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2996,8 +2996,8 @@
   <sheetPr/>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -3027,7 +3027,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -3037,7 +3037,7 @@
         <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -3047,7 +3047,7 @@
         <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -3057,7 +3057,7 @@
         <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
@@ -3067,7 +3067,7 @@
         <v>126</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -3077,7 +3077,7 @@
         <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
@@ -3087,7 +3087,7 @@
         <v>128</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -3097,7 +3097,7 @@
         <v>129</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -3107,7 +3107,7 @@
         <v>130</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
@@ -3117,7 +3117,7 @@
         <v>131</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
@@ -3127,7 +3127,7 @@
         <v>132</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -3137,7 +3137,7 @@
         <v>133</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>134</v>
@@ -3151,7 +3151,7 @@
         <v>136</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>137</v>
@@ -3165,7 +3165,7 @@
         <v>138</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>139</v>
@@ -3179,7 +3179,7 @@
         <v>141</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>142</v>
@@ -3193,7 +3193,7 @@
         <v>144</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>145</v>
@@ -3207,7 +3207,7 @@
         <v>146</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
@@ -3217,7 +3217,7 @@
         <v>147</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
@@ -3227,7 +3227,7 @@
         <v>148</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
@@ -3237,7 +3237,7 @@
         <v>149</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
@@ -3247,7 +3247,7 @@
         <v>150</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>61</v>
@@ -3261,7 +3261,7 @@
         <v>151</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>61</v>
@@ -3275,7 +3275,7 @@
         <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
some fixes for ListinInfoClassifiedTest done
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="786" firstSheet="6" activeTab="7"/>
+    <workbookView windowWidth="28000" windowHeight="10960" tabRatio="928" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralConfig" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204">
   <si>
     <t>Parameters</t>
   </si>
@@ -149,6 +149,9 @@
     <t>verifyNewOpportunityNavigation</t>
   </si>
   <si>
+    <t>skip</t>
+  </si>
+  <si>
     <t>verifyNewOpportunityHeaderLabel</t>
   </si>
   <si>
@@ -221,9 +224,6 @@
     <t>verifyNewOpportunity</t>
   </si>
   <si>
-    <t>skip</t>
-  </si>
-  <si>
     <t>verifyOpportunities</t>
   </si>
   <si>
@@ -338,7 +338,7 @@
     <t>CreateOpportunityForClassified</t>
   </si>
   <si>
-    <t>AJ Pointon &amp; AW Pointon,10,Cattle,Buffalo,Angus,$/head,10,2,5,Month,Test,Test</t>
+    <t>BR&amp;C Consignment Stock - GST,10,Cattle,Bull,Angus,$/head,10,2,5,Month,Test,Test</t>
   </si>
   <si>
     <t>vendorName,quantity,productCategory,product,breed,priceType,price,age1,age2,monthsDropdown,description,noteText</t>
@@ -347,204 +347,204 @@
     <t>verifyListingTypeSelectionClassified</t>
   </si>
   <si>
+    <t>verifyListingInfoNavigationClassified</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedListingOverviewDetails</t>
+  </si>
+  <si>
+    <t>14 days,150,Test Description,AARONS</t>
+  </si>
+  <si>
+    <t>classifiedDuration,price,description</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedLotDetails</t>
+  </si>
+  <si>
+    <t>Polled,10,20</t>
+  </si>
+  <si>
+    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
+  </si>
+  <si>
+    <t>verifyFillingClassifiedHealthVetDetails</t>
+  </si>
+  <si>
+    <t>verifyClassifiedPublishListing</t>
+  </si>
+  <si>
+    <t>verifyOpportunityIdNavigationFromGridPage</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigationFromListingPage</t>
+  </si>
+  <si>
+    <t>verifyFillingNewContract</t>
+  </si>
+  <si>
+    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
+  </si>
+  <si>
+    <t>salesType,branchName,buyerName,deliveryPoint</t>
+  </si>
+  <si>
+    <t>verifyNewContractNavigation</t>
+  </si>
+  <si>
+    <t>verifyNewContractHeaderLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractSalesInformationLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractVendorInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyBuyerInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyDeliveryInfoLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractLotsLabel</t>
+  </si>
+  <si>
+    <t>verifyAdditionalChargesLabel</t>
+  </si>
+  <si>
+    <t>verifyCommissionAndAgentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotesLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachmentsLabel</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddSalesInformation</t>
+  </si>
+  <si>
+    <t>Dairy,ALBANY,June,8,2020</t>
+  </si>
+  <si>
+    <t>salesType,branchName,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddVendorInfo</t>
+  </si>
+  <si>
+    <t>Corrigin Cash account</t>
+  </si>
+  <si>
+    <t>verifyAddBuyerInfo</t>
+  </si>
+  <si>
+    <t>Chatley &amp; Hutcheson</t>
+  </si>
+  <si>
+    <t>buyerName</t>
+  </si>
+  <si>
+    <t>verifyAddDeliveryInfo</t>
+  </si>
+  <si>
+    <t>Test Delivery Point,June,12,2020</t>
+  </si>
+  <si>
+    <t>deliveryPoint,month,day,year</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddLotsInfo</t>
+  </si>
+  <si>
+    <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
+  </si>
+  <si>
+    <t>verifyAddAdditionalCharges</t>
+  </si>
+  <si>
+    <t>verifyAddCommissionAndAgents</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddAttachments</t>
+  </si>
+  <si>
+    <t>verifyNewContractAttachments</t>
+  </si>
+  <si>
+    <t>verifyNewContractAddNotes</t>
+  </si>
+  <si>
+    <t>verifyNewContractNotes</t>
+  </si>
+  <si>
+    <t>verifyValidateContract</t>
+  </si>
+  <si>
+    <t>Ashish,Test Buyer,Test Vendor</t>
+  </si>
+  <si>
+    <t>agentSignature,buyerSignature,VendorSignature</t>
+  </si>
+  <si>
+    <t>VerifyAddingSalesAndVendorInfo</t>
+  </si>
+  <si>
+    <t>A Rigano</t>
+  </si>
+  <si>
+    <t>verifyPerKGConditionInLot</t>
+  </si>
+  <si>
+    <t>15,Sheep,Ewe,Bond</t>
+  </si>
+  <si>
+    <t>quantity,productCategory,product,breed</t>
+  </si>
+  <si>
+    <t>verifyAddingValueToPerKGFieldInLot</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>verifyWeightValueOnLotGridPage</t>
+  </si>
+  <si>
+    <t>quantity,weight</t>
+  </si>
+  <si>
+    <t>verifyAddingSecondLotInTheSameOpportunity</t>
+  </si>
+  <si>
+    <t>10,Cattle,Buffalo,Angus</t>
+  </si>
+  <si>
+    <t>verifyDisabledListingType</t>
+  </si>
+  <si>
+    <t>VerifyEditingLotsInfo</t>
+  </si>
+  <si>
+    <t>Cheviot</t>
+  </si>
+  <si>
+    <t>updatedBreed</t>
+  </si>
+  <si>
+    <t>VerifyDeletingLot</t>
+  </si>
+  <si>
+    <t>verifyEnabledListingType</t>
+  </si>
+  <si>
+    <t>verifyBidAndOfferListingTypeSelection</t>
+  </si>
+  <si>
     <t>Online,Dairy</t>
   </si>
   <si>
-    <t>verifyListingInfoNavigationClassified</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedListingOverviewDetails</t>
-  </si>
-  <si>
-    <t>14 days,150,Test Description</t>
-  </si>
-  <si>
-    <t>classifiedDuration,price,description</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedLotDetails</t>
-  </si>
-  <si>
-    <t>Polled,10,20</t>
-  </si>
-  <si>
-    <t>hornStatus,weightRangeLow,weightRangeHigh</t>
-  </si>
-  <si>
-    <t>verifyFillingClassifiedHealthVetDetails</t>
-  </si>
-  <si>
-    <t>verifyClassifiedPublishListing</t>
-  </si>
-  <si>
-    <t>verifyOpportunityIdNavigationFromGridPage</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigationFromListingPage</t>
-  </si>
-  <si>
-    <t>verifyFillingNewContract</t>
-  </si>
-  <si>
-    <t>Agent settlement,Alexandra,AJ Pointon &amp; AW Pointon,Test Point</t>
-  </si>
-  <si>
-    <t>salesType,branchName,buyerName,deliveryPoint</t>
-  </si>
-  <si>
-    <t>verifyNewContractNavigation</t>
-  </si>
-  <si>
-    <t>verifyNewContractHeaderLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractSalesInformationLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractVendorInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyBuyerInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyDeliveryInfoLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractLotsLabel</t>
-  </si>
-  <si>
-    <t>verifyAdditionalChargesLabel</t>
-  </si>
-  <si>
-    <t>verifyCommissionAndAgentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotesLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachmentsLabel</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddSalesInformation</t>
-  </si>
-  <si>
-    <t>Dairy,ALBANY,June,8,2020</t>
-  </si>
-  <si>
-    <t>salesType,branchName,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddVendorInfo</t>
-  </si>
-  <si>
-    <t>Corrigin Cash account</t>
-  </si>
-  <si>
-    <t>verifyAddBuyerInfo</t>
-  </si>
-  <si>
-    <t>Chatley &amp; Hutcheson</t>
-  </si>
-  <si>
-    <t>buyerName</t>
-  </si>
-  <si>
-    <t>verifyAddDeliveryInfo</t>
-  </si>
-  <si>
-    <t>Test Delivery Point,June,12,2020</t>
-  </si>
-  <si>
-    <t>deliveryPoint,month,day,year</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddLotsInfo</t>
-  </si>
-  <si>
-    <t>10,Sheep,Eve,Bond,$/head,10,2,5,Month,Test</t>
-  </si>
-  <si>
-    <t>verifyAddAdditionalCharges</t>
-  </si>
-  <si>
-    <t>verifyAddCommissionAndAgents</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddAttachments</t>
-  </si>
-  <si>
-    <t>verifyNewContractAttachments</t>
-  </si>
-  <si>
-    <t>verifyNewContractAddNotes</t>
-  </si>
-  <si>
-    <t>verifyNewContractNotes</t>
-  </si>
-  <si>
-    <t>verifyValidateContract</t>
-  </si>
-  <si>
-    <t>Ashish,Test Buyer,Test Vendor</t>
-  </si>
-  <si>
-    <t>agentSignature,buyerSignature,VendorSignature</t>
-  </si>
-  <si>
-    <t>VerifyAddingSalesAndVendorInfo</t>
-  </si>
-  <si>
-    <t>A Rigano</t>
-  </si>
-  <si>
-    <t>verifyPerKGConditionInLot</t>
-  </si>
-  <si>
-    <t>15,Sheep,Ewe,Bond</t>
-  </si>
-  <si>
-    <t>quantity,productCategory,product,breed</t>
-  </si>
-  <si>
-    <t>verifyAddingValueToPerKGFieldInLot</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>verifyWeightValueOnLotGridPage</t>
-  </si>
-  <si>
-    <t>quantity,weight</t>
-  </si>
-  <si>
-    <t>verifyAddingSecondLotInTheSameOpportunity</t>
-  </si>
-  <si>
-    <t>10,Cattle,Buffalo,Angus</t>
-  </si>
-  <si>
-    <t>verifyDisabledListingType</t>
-  </si>
-  <si>
-    <t>VerifyEditingLotsInfo</t>
-  </si>
-  <si>
-    <t>Cheviot</t>
-  </si>
-  <si>
-    <t>updatedBreed</t>
-  </si>
-  <si>
-    <t>VerifyDeletingLot</t>
-  </si>
-  <si>
-    <t>verifyEnabledListingType</t>
-  </si>
-  <si>
-    <t>verifyBidAndOfferListingTypeSelection</t>
-  </si>
-  <si>
     <t>verifyFillingListingOverviewDetailsForSheep</t>
   </si>
   <si>
@@ -621,9 +621,6 @@
   </si>
   <si>
     <t>verifyFillingClassifiedListingOverviewDetailsSheep</t>
-  </si>
-  <si>
-    <t>14 days,150,Test Description,AARONS</t>
   </si>
   <si>
     <t>classifiedDuration,price,description,town</t>
@@ -646,10 +643,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -701,16 +698,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -725,31 +730,31 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -764,6 +769,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -771,7 +790,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -785,24 +804,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -810,13 +813,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -830,8 +826,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -846,7 +843,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,19 +963,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,127 +1005,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,19 +1023,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,32 +1061,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1108,8 +1079,49 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,8 +1129,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1137,162 +1149,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1926,13 +1923,13 @@
     </row>
     <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
@@ -1943,7 +1940,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>174</v>
@@ -1957,7 +1954,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>84</v>
@@ -1971,7 +1968,7 @@
         <v>176</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>177</v>
@@ -1985,7 +1982,7 @@
         <v>179</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>180</v>
@@ -1999,7 +1996,7 @@
         <v>182</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>183</v>
@@ -2013,7 +2010,7 @@
         <v>185</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>186</v>
@@ -2027,7 +2024,7 @@
         <v>188</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2041,7 +2038,7 @@
         <v>190</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:2">
@@ -2049,7 +2046,7 @@
         <v>191</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:2">
@@ -2057,7 +2054,7 @@
         <v>192</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="1:3">
@@ -2065,7 +2062,7 @@
         <v>193</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>194</v>
@@ -2076,7 +2073,7 @@
         <v>195</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +2088,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2121,7 +2118,7 @@
         <v>196</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2131,7 +2128,7 @@
         <v>197</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2141,53 +2138,53 @@
         <v>198</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="15.75" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -2203,7 +2200,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2258,7 +2255,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2286,179 +2283,179 @@
         <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2500,10 +2497,10 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2513,7 +2510,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2523,7 +2520,7 @@
         <v>67</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2533,7 +2530,7 @@
         <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
@@ -2543,7 +2540,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -2553,7 +2550,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
@@ -2563,7 +2560,7 @@
         <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -2573,7 +2570,7 @@
         <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
@@ -2590,7 +2587,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2620,7 +2617,7 @@
         <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
@@ -2630,7 +2627,7 @@
         <v>74</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
@@ -2640,7 +2637,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
@@ -2650,7 +2647,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>77</v>
@@ -2664,7 +2661,7 @@
         <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
@@ -2674,7 +2671,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>81</v>
@@ -2688,7 +2685,7 @@
         <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>84</v>
@@ -2702,7 +2699,7 @@
         <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>87</v>
@@ -2716,7 +2713,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>90</v>
@@ -2730,7 +2727,7 @@
         <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>93</v>
@@ -2744,7 +2741,7 @@
         <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
@@ -2754,7 +2751,7 @@
         <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>97</v>
@@ -2768,7 +2765,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>100</v>
@@ -2782,7 +2779,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="3"/>
@@ -2798,8 +2795,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -2829,7 +2826,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>104</v>
@@ -2843,10 +2840,10 @@
         <v>106</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>78</v>
@@ -2854,48 +2851,48 @@
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>93</v>
@@ -2906,10 +2903,10 @@
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
@@ -2953,36 +2950,36 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2996,8 +2993,8 @@
   <sheetPr/>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -3024,264 +3021,264 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" ht="14.8" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" ht="14.8" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="14.8" spans="1:4">
       <c r="A13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" ht="14.8" spans="1:4">
       <c r="A14" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" ht="14.8" spans="1:4">
       <c r="A15" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" ht="14.8" spans="1:4">
       <c r="A16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="17" ht="14.8" spans="1:4">
       <c r="A17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" ht="14.8" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" ht="14.8" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" ht="14.8" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" ht="14.8" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" ht="14.8" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" ht="14.8" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" ht="14.8" spans="1:4">
       <c r="A24" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3323,114 +3320,114 @@
     </row>
     <row r="2" ht="14.8" spans="1:4">
       <c r="A2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="14.8" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="4" ht="14.8" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3">
         <v>900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" ht="14.8" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5">
         <v>900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" ht="14.8" spans="1:4">
       <c r="A6" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" ht="14.8" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="14.8" spans="1:4">
       <c r="A8" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="9" ht="14.8" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="14.8" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>